<commit_message>
new help pages - account / custom data, admin / users, roles
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@54391 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="134">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -108,15 +108,9 @@
     <t xml:space="preserve">Bandwidth usage </t>
   </si>
   <si>
-    <t xml:space="preserve">content report </t>
-  </si>
-  <si>
     <t xml:space="preserve">users &amp; community </t>
   </si>
   <si>
-    <t xml:space="preserve">manage </t>
-  </si>
-  <si>
     <t>users</t>
   </si>
   <si>
@@ -235,13 +229,202 @@
   </si>
   <si>
     <t>roles</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>topContet</t>
+  </si>
+  <si>
+    <t>contentDropOff</t>
+  </si>
+  <si>
+    <t>contentInteractions</t>
+  </si>
+  <si>
+    <t>contentContributions</t>
+  </si>
+  <si>
+    <t>videoDrillDownDefault</t>
+  </si>
+  <si>
+    <t>videoDrillDownDropoff</t>
+  </si>
+  <si>
+    <t>contentContributionsDrillDown</t>
+  </si>
+  <si>
+    <t>content reports</t>
+  </si>
+  <si>
+    <t>analytics.view.Users.mxml</t>
+  </si>
+  <si>
+    <t>topContributors</t>
+  </si>
+  <si>
+    <t>mapOverlay</t>
+  </si>
+  <si>
+    <t>topSyndications</t>
+  </si>
+  <si>
+    <t>syndicationsDrillDown</t>
+  </si>
+  <si>
+    <t>mapOverlayDrillDown</t>
+  </si>
+  <si>
+    <t>administration</t>
+  </si>
+  <si>
+    <t>section1</t>
+  </si>
+  <si>
+    <t>section2</t>
+  </si>
+  <si>
+    <t>section3</t>
+  </si>
+  <si>
+    <t>section4</t>
+  </si>
+  <si>
+    <t>section5</t>
+  </si>
+  <si>
+    <t>section6</t>
+  </si>
+  <si>
+    <t>section7</t>
+  </si>
+  <si>
+    <t>section8</t>
+  </si>
+  <si>
+    <t>section9</t>
+  </si>
+  <si>
+    <t>section10</t>
+  </si>
+  <si>
+    <t>section11</t>
+  </si>
+  <si>
+    <t>section12</t>
+  </si>
+  <si>
+    <t>section13</t>
+  </si>
+  <si>
+    <t>section14</t>
+  </si>
+  <si>
+    <t>section15</t>
+  </si>
+  <si>
+    <t>section16</t>
+  </si>
+  <si>
+    <t>section17</t>
+  </si>
+  <si>
+    <t>section18</t>
+  </si>
+  <si>
+    <t>section19</t>
+  </si>
+  <si>
+    <t>section20</t>
+  </si>
+  <si>
+    <t>section21</t>
+  </si>
+  <si>
+    <t>section22</t>
+  </si>
+  <si>
+    <t>section23</t>
+  </si>
+  <si>
+    <t>section24</t>
+  </si>
+  <si>
+    <t>section25</t>
+  </si>
+  <si>
+    <t>section26</t>
+  </si>
+  <si>
+    <t>section27</t>
+  </si>
+  <si>
+    <t>section28</t>
+  </si>
+  <si>
+    <t>section29</t>
+  </si>
+  <si>
+    <t>section30</t>
+  </si>
+  <si>
+    <t>section31</t>
+  </si>
+  <si>
+    <t>section32</t>
+  </si>
+  <si>
+    <t>section33</t>
+  </si>
+  <si>
+    <t>section34</t>
+  </si>
+  <si>
+    <t>section35</t>
+  </si>
+  <si>
+    <t>section36</t>
+  </si>
+  <si>
+    <t>section37</t>
+  </si>
+  <si>
+    <t>section38</t>
+  </si>
+  <si>
+    <t>section39</t>
+  </si>
+  <si>
+    <t>section40</t>
+  </si>
+  <si>
+    <t>section41</t>
+  </si>
+  <si>
+    <t>section42</t>
+  </si>
+  <si>
+    <t>section43</t>
+  </si>
+  <si>
+    <t>section44</t>
+  </si>
+  <si>
+    <t>section45</t>
+  </si>
+  <si>
+    <t>videoDrillDownInteractions</t>
+  </si>
+  <si>
+    <t>section46</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,8 +456,16 @@
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +489,11 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -308,11 +504,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -323,8 +520,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -618,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C54" activeCellId="1" sqref="C52 C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -638,45 +841,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>52</v>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>44</v>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -684,349 +887,515 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>45</v>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>67</v>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>68</v>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>46</v>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>11</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B16">
-        <v>12</v>
-      </c>
-      <c r="C16" s="4" t="s">
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>49</v>
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18">
-      <c r="A24" s="2" t="s">
-        <v>18</v>
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18">
+      <c r="A23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25">
-        <v>15</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>41</v>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26">
-        <v>16</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="18">
-      <c r="A29" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30">
-        <v>17</v>
-      </c>
-      <c r="C30" s="4" t="s">
         <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31">
-        <v>19</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32">
-        <v>20</v>
-      </c>
-      <c r="C32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33">
-        <v>21</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>39</v>
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="18">
+      <c r="A33" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34">
-        <v>22</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>59</v>
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35">
-        <v>23</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>66</v>
+      <c r="A35" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36">
-        <v>24</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>69</v>
+      <c r="A36" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37">
-        <v>25</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
+      </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38">
-        <v>26</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="18">
-      <c r="A40" s="2" t="s">
-        <v>28</v>
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41">
-        <v>27</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>53</v>
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15">
+      <c r="A44" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B42">
-        <v>28</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" ht="15">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" ht="15">
+      <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" ht="15">
+      <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" ht="15">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" ht="15">
+      <c r="A49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" ht="18">
+      <c r="A50" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15">
-      <c r="A43" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43">
-        <v>29</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="45" spans="1:5" ht="18">
-      <c r="A45" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46">
-        <v>30</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47">
-        <v>31</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48">
-        <v>32</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49">
-        <v>33</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fwr: bulk uploads in "upload" menu
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@81467 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="20775" windowHeight="13410"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1255,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fwr: updates to help anchors
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@81554 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="330">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -744,9 +744,6 @@
     <t>Nethelp - dz</t>
   </si>
   <si>
-    <t>mediamanagementandwo.htm</t>
-  </si>
-  <si>
     <t>editentrymenus.htm</t>
   </si>
   <si>
@@ -759,9 +756,6 @@
     <t>addingcaptionstoanen.htm</t>
   </si>
   <si>
-    <t>is this available dz</t>
-  </si>
-  <si>
     <t>legacy dz</t>
   </si>
   <si>
@@ -813,9 +807,6 @@
     <t>addingmetadatatoacat.htm</t>
   </si>
   <si>
-    <t>contentprivacy.htm</t>
-  </si>
-  <si>
     <t>playerlist.htm</t>
   </si>
   <si>
@@ -916,6 +907,105 @@
   </si>
   <si>
     <t>&lt;/help&gt;</t>
+  </si>
+  <si>
+    <t>entriestab.htm</t>
+  </si>
+  <si>
+    <t>dz could not access - after creating clip</t>
+  </si>
+  <si>
+    <t>replacingmedia.htm</t>
+  </si>
+  <si>
+    <t>dz could not create - ls still provistioning</t>
+  </si>
+  <si>
+    <t>userstab.htm</t>
+  </si>
+  <si>
+    <t>downloadfiles.htm</t>
+  </si>
+  <si>
+    <t>addtags1.htm</t>
+  </si>
+  <si>
+    <t>removingtags.htm</t>
+  </si>
+  <si>
+    <t>setaccesscontrol.htm</t>
+  </si>
+  <si>
+    <t>setscheduling.htm</t>
+  </si>
+  <si>
+    <t>changeowner1.htm</t>
+  </si>
+  <si>
+    <t>removecategories.htm</t>
+  </si>
+  <si>
+    <t>creatingalivestreami.htm</t>
+  </si>
+  <si>
+    <t>matchfilesfromdropfo.htm</t>
+  </si>
+  <si>
+    <t>addvideoaudio.htm</t>
+  </si>
+  <si>
+    <t>dz- could not create</t>
+  </si>
+  <si>
+    <t>themoderatationtab.htm</t>
+  </si>
+  <si>
+    <t>thecategoriestab.htm</t>
+  </si>
+  <si>
+    <t>categoryenduseracces.htm</t>
+  </si>
+  <si>
+    <t>subcategories.htm</t>
+  </si>
+  <si>
+    <t>enduseraccesspermiss.htm</t>
+  </si>
+  <si>
+    <t>addinguserpermission.htm</t>
+  </si>
+  <si>
+    <t>addtags.htm</t>
+  </si>
+  <si>
+    <t>removetags.htm</t>
+  </si>
+  <si>
+    <t>movecategories.htm</t>
+  </si>
+  <si>
+    <t>changelisting.htm</t>
+  </si>
+  <si>
+    <t>changeaccess.htm</t>
+  </si>
+  <si>
+    <t>changeowner.htm</t>
+  </si>
+  <si>
+    <t>youruploads.htm</t>
+  </si>
+  <si>
+    <t>bulkuploadlog.htm</t>
+  </si>
+  <si>
+    <t>usingadropfolder.htm</t>
+  </si>
+  <si>
+    <t>addingentitlementcon.htm</t>
+  </si>
+  <si>
+    <t>&lt;help&gt;</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1124,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1053,6 +1143,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1360,13 +1451,13 @@
   <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H104"/>
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="7" customWidth="1"/>
   </cols>
@@ -1390,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>299</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1398,7 +1489,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>242</v>
+        <v>297</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>74</v>
@@ -1408,7 +1499,7 @@
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("&lt;item key=""",C3,""" anchor=""",B3,""" /&gt;")</f>
-        <v>&lt;item key="section_entries" anchor="mediamanagementandwo.htm" /&gt;</v>
+        <v>&lt;item key="section_entries" anchor="entriestab.htm" /&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1416,7 +1507,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>37</v>
@@ -1431,7 +1522,7 @@
         <v>183</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>167</v>
@@ -1449,7 +1540,7 @@
         <v>181</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>168</v>
@@ -1467,7 +1558,7 @@
         <v>182</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>169</v>
@@ -1485,7 +1576,7 @@
         <v>184</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>247</v>
+        <v>298</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>170</v>
@@ -1495,7 +1586,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_clips" anchor="is this available dz" /&gt;</v>
+        <v>&lt;item key="entry_clips" anchor="dz could not access - after creating clip" /&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1503,7 +1594,7 @@
         <v>185</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>171</v>
@@ -1521,7 +1612,7 @@
         <v>186</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>172</v>
@@ -1539,7 +1630,7 @@
         <v>187</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>173</v>
@@ -1557,7 +1648,7 @@
         <v>188</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>174</v>
@@ -1574,6 +1665,9 @@
       <c r="A13" t="s">
         <v>176</v>
       </c>
+      <c r="B13" s="5" t="s">
+        <v>299</v>
+      </c>
       <c r="C13" s="5" t="s">
         <v>175</v>
       </c>
@@ -1582,13 +1676,16 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_replacement" anchor="" /&gt;</v>
+        <v>&lt;item key="entry_replacement" anchor="replacingmedia.htm" /&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>188</v>
       </c>
+      <c r="B14" s="11" t="s">
+        <v>300</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>85</v>
       </c>
@@ -1597,7 +1694,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_live_stream" anchor="" /&gt;</v>
+        <v>&lt;item key="section_live_stream" anchor="dz could not create - ls still provistioning" /&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1605,7 +1702,7 @@
         <v>189</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>177</v>
@@ -1623,7 +1720,7 @@
         <v>190</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>178</v>
@@ -1641,7 +1738,7 @@
         <v>191</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>179</v>
@@ -1658,6 +1755,9 @@
       <c r="A18" t="s">
         <v>192</v>
       </c>
+      <c r="B18" s="5" t="s">
+        <v>301</v>
+      </c>
       <c r="C18" s="5" t="s">
         <v>180</v>
       </c>
@@ -1666,13 +1766,16 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_users" anchor="" /&gt;</v>
+        <v>&lt;item key="entry_users" anchor="userstab.htm" /&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>193</v>
       </c>
+      <c r="B19" s="5" t="s">
+        <v>302</v>
+      </c>
       <c r="C19" s="5" t="s">
         <v>117</v>
       </c>
@@ -1682,13 +1785,16 @@
       <c r="F19" s="3"/>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_download" anchor="" /&gt;</v>
+        <v>&lt;item key="section_download" anchor="downloadfiles.htm" /&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>194</v>
       </c>
+      <c r="B20" s="5" t="s">
+        <v>303</v>
+      </c>
       <c r="C20" s="5" t="s">
         <v>114</v>
       </c>
@@ -1697,13 +1803,16 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_entry_tags" anchor="" /&gt;</v>
+        <v>&lt;item key="section_add_entry_tags" anchor="addtags1.htm" /&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>195</v>
       </c>
+      <c r="B21" s="5" t="s">
+        <v>304</v>
+      </c>
       <c r="C21" s="5" t="s">
         <v>118</v>
       </c>
@@ -1712,13 +1821,16 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_remove_entry_tags" anchor="" /&gt;</v>
+        <v>&lt;item key="section_remove_entry_tags" anchor="removingtags.htm" /&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>196</v>
       </c>
+      <c r="B22" s="5" t="s">
+        <v>305</v>
+      </c>
       <c r="C22" s="5" t="s">
         <v>120</v>
       </c>
@@ -1727,13 +1839,16 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_access_control" anchor="" /&gt;</v>
+        <v>&lt;item key="section_bulk_access_control" anchor="setaccesscontrol.htm" /&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>197</v>
       </c>
+      <c r="B23" s="5" t="s">
+        <v>306</v>
+      </c>
       <c r="C23" s="5" t="s">
         <v>121</v>
       </c>
@@ -1742,13 +1857,16 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_sched" anchor="" /&gt;</v>
+        <v>&lt;item key="section_bulk_sched" anchor="setscheduling.htm" /&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>221</v>
       </c>
+      <c r="B24" s="5" t="s">
+        <v>307</v>
+      </c>
       <c r="C24" s="5" t="s">
         <v>220</v>
       </c>
@@ -1757,13 +1875,16 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entry_owner" anchor="" /&gt;</v>
+        <v>&lt;item key="section_entry_owner" anchor="changeowner1.htm" /&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>225</v>
       </c>
+      <c r="B25" s="5" t="s">
+        <v>308</v>
+      </c>
       <c r="C25" s="5" t="s">
         <v>223</v>
       </c>
@@ -1772,14 +1893,16 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entry_remove_cats" anchor="" /&gt;</v>
+        <v>&lt;item key="section_entry_remove_cats" anchor="removecategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="C26" s="5" t="s">
         <v>113</v>
       </c>
@@ -1788,14 +1911,16 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_live_stream" anchor="" /&gt;</v>
+        <v>&lt;item key="section_add_live_stream" anchor="creatingalivestreami.htm" /&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>157</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="C27" s="5" t="s">
         <v>155</v>
       </c>
@@ -1804,7 +1929,7 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_dropfolder" anchor="" /&gt;</v>
+        <v>&lt;item key="section_flavor_dropfolder" anchor="matchfilesfromdropfo.htm" /&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1812,7 +1937,7 @@
         <v>161</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>158</v>
@@ -1829,7 +1954,9 @@
       <c r="A29" t="s">
         <v>163</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>159</v>
       </c>
@@ -1838,14 +1965,16 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_import" anchor="" /&gt;</v>
+        <v>&lt;item key="section_flavor_import" anchor="addvideoaudio.htm" /&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="6"/>
+      <c r="B30" s="12" t="s">
+        <v>312</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>160</v>
       </c>
@@ -1854,13 +1983,16 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_link" anchor="" /&gt;</v>
+        <v>&lt;item key="section_flavor_link" anchor="dz- could not create" /&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B31" s="5" t="s">
+        <v>313</v>
+      </c>
       <c r="C31" s="5" t="s">
         <v>75</v>
       </c>
@@ -1869,7 +2001,7 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_moderation" anchor="" /&gt;</v>
+        <v>&lt;item key="section_moderation" anchor="themoderatationtab.htm" /&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1877,7 +2009,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>76</v>
@@ -1895,7 +2027,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>83</v>
@@ -1913,7 +2045,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>119</v>
@@ -1931,7 +2063,7 @@
         <v>24</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>112</v>
@@ -1948,6 +2080,9 @@
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B36" s="5" t="s">
+        <v>259</v>
+      </c>
       <c r="C36" s="5" t="s">
         <v>77</v>
       </c>
@@ -1956,15 +2091,15 @@
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_syndication" anchor="" /&gt;</v>
+        <v>&lt;item key="section_syndication" anchor="settingupsyndication.htm" /&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>111</v>
@@ -1982,7 +2117,7 @@
         <v>11</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>110</v>
@@ -1999,7 +2134,9 @@
       <c r="A39" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B39" s="6"/>
+      <c r="B39" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="C39" s="5" t="s">
         <v>165</v>
       </c>
@@ -2008,7 +2145,7 @@
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_categories" anchor="" /&gt;</v>
+        <v>&lt;item key="section_categories" anchor="thecategoriestab.htm" /&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2016,7 +2153,7 @@
         <v>199</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>198</v>
@@ -2034,7 +2171,7 @@
         <v>200</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>205</v>
@@ -2052,7 +2189,7 @@
         <v>201</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>265</v>
+        <v>315</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>204</v>
@@ -2062,14 +2199,16 @@
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_users" anchor="contentprivacy.htm" /&gt;</v>
+        <v>&lt;item key="section_category_users" anchor="categoryenduseracces.htm" /&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B43" s="6"/>
+      <c r="B43" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="C43" s="5" t="s">
         <v>206</v>
       </c>
@@ -2078,14 +2217,16 @@
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_subcats" anchor="" /&gt;</v>
+        <v>&lt;item key="section_category_subcats" anchor="subcategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B44" s="6"/>
+      <c r="B44" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="C44" s="5" t="s">
         <v>209</v>
       </c>
@@ -2094,14 +2235,16 @@
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_permission" anchor="" /&gt;</v>
+        <v>&lt;item key="section_cat_user_permission" anchor="enduseraccesspermiss.htm" /&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B45" s="6"/>
+      <c r="B45" s="6" t="s">
+        <v>261</v>
+      </c>
       <c r="C45" s="6" t="s">
         <v>210</v>
       </c>
@@ -2110,14 +2253,16 @@
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_add" anchor="" /&gt;</v>
+        <v>&lt;item key="section_cat_user_add" anchor="addacategory.htm" /&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B46" s="6"/>
+      <c r="B46" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="C46" s="6" t="s">
         <v>214</v>
       </c>
@@ -2126,14 +2271,16 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_cat_user_permission" anchor="" /&gt;</v>
+        <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B47" s="6"/>
+      <c r="B47" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="C47" s="6" t="s">
         <v>216</v>
       </c>
@@ -2142,14 +2289,16 @@
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_cat_tags" anchor="" /&gt;</v>
+        <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B48" s="6"/>
+      <c r="B48" s="6" t="s">
+        <v>320</v>
+      </c>
       <c r="C48" s="6" t="s">
         <v>218</v>
       </c>
@@ -2158,14 +2307,16 @@
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_remove_cat_tags" anchor="" /&gt;</v>
+        <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B49" s="6"/>
+      <c r="B49" s="6" t="s">
+        <v>321</v>
+      </c>
       <c r="C49" s="6" t="s">
         <v>226</v>
       </c>
@@ -2174,14 +2325,16 @@
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_move" anchor="" /&gt;</v>
+        <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B50" s="6"/>
+      <c r="B50" s="6" t="s">
+        <v>322</v>
+      </c>
       <c r="C50" s="6" t="s">
         <v>229</v>
       </c>
@@ -2190,14 +2343,16 @@
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_list" anchor="" /&gt;</v>
+        <v>&lt;item key="section_cats_list" anchor="changelisting.htm" /&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B51" s="6"/>
+      <c r="B51" s="6" t="s">
+        <v>323</v>
+      </c>
       <c r="C51" s="6" t="s">
         <v>231</v>
       </c>
@@ -2206,14 +2361,16 @@
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_access" anchor="" /&gt;</v>
+        <v>&lt;item key="section_cats_access" anchor="changeaccess.htm" /&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B52" s="6"/>
+      <c r="B52" s="6" t="s">
+        <v>324</v>
+      </c>
       <c r="C52" s="6" t="s">
         <v>233</v>
       </c>
@@ -2222,7 +2379,7 @@
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_owner" anchor="" /&gt;</v>
+        <v>&lt;item key="section_cats_owner" anchor="changeowner.htm" /&gt;</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2249,6 +2406,9 @@
       <c r="A55" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B55" s="5" t="s">
+        <v>325</v>
+      </c>
       <c r="C55" s="5" t="s">
         <v>78</v>
       </c>
@@ -2257,13 +2417,16 @@
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_uploads" anchor="" /&gt;</v>
+        <v>&lt;item key="section_uploads" anchor="youruploads.htm" /&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="B56" s="5" t="s">
+        <v>326</v>
+      </c>
       <c r="C56" s="5" t="s">
         <v>80</v>
       </c>
@@ -2272,13 +2435,16 @@
       </c>
       <c r="H56" t="str">
         <f>CONCATENATE("&lt;item key=""",C56,""" anchor=""",B56,""" /&gt;")</f>
-        <v>&lt;item key="section_bulk_log" anchor="" /&gt;</v>
+        <v>&lt;item key="section_bulk_log" anchor="bulkuploadlog.htm" /&gt;</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="B57" s="5" t="s">
+        <v>327</v>
+      </c>
       <c r="C57" s="5" t="s">
         <v>81</v>
       </c>
@@ -2287,7 +2453,7 @@
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_drop_folders" anchor="" /&gt;</v>
+        <v>&lt;item key="section_drop_folders" anchor="usingadropfolder.htm" /&gt;</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="18.75">
@@ -2304,7 +2470,7 @@
         <v>13</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>122</v>
@@ -2322,7 +2488,7 @@
         <v>124</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>123</v>
@@ -2349,7 +2515,7 @@
         <v>15</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>125</v>
@@ -2367,7 +2533,7 @@
         <v>17</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>126</v>
@@ -2384,6 +2550,9 @@
       <c r="A64" t="s">
         <v>154</v>
       </c>
+      <c r="B64" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="C64" s="5" t="s">
         <v>153</v>
       </c>
@@ -2392,13 +2561,16 @@
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entitlement_more" anchor="" /&gt;</v>
+        <v>&lt;item key="section_entitlement_more" anchor="section_entitlement_more" /&gt;</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>240</v>
       </c>
+      <c r="B65" s="5" t="s">
+        <v>328</v>
+      </c>
       <c r="C65" s="5" t="s">
         <v>238</v>
       </c>
@@ -2407,7 +2579,7 @@
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_entitlement" anchor="" /&gt;</v>
+        <v>&lt;item key="section_cat_entitlement" anchor="addingentitlementcon.htm" /&gt;</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2415,7 +2587,7 @@
         <v>16</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>127</v>
@@ -2433,7 +2605,7 @@
         <v>18</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>84</v>
@@ -2451,7 +2623,7 @@
         <v>129</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>128</v>
@@ -2469,7 +2641,7 @@
         <v>130</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>131</v>
@@ -2487,7 +2659,7 @@
         <v>142</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>143</v>
@@ -2505,7 +2677,7 @@
         <v>141</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>139</v>
@@ -2523,7 +2695,7 @@
         <v>48</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>132</v>
@@ -2541,7 +2713,7 @@
         <v>144</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="8" t="s">
@@ -2557,7 +2729,7 @@
         <v>87</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>86</v>
@@ -2575,7 +2747,7 @@
         <v>43</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>133</v>
@@ -2593,7 +2765,7 @@
         <v>135</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>134</v>
@@ -2620,7 +2792,7 @@
         <v>20</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>100</v>
@@ -2647,7 +2819,7 @@
         <v>57</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>92</v>
@@ -2665,7 +2837,7 @@
         <v>58</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>93</v>
@@ -2683,7 +2855,7 @@
         <v>59</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>94</v>
@@ -2701,7 +2873,7 @@
         <v>60</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>95</v>
@@ -2719,7 +2891,7 @@
         <v>61</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>96</v>
@@ -2737,7 +2909,7 @@
         <v>62</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>97</v>
@@ -2755,7 +2927,7 @@
         <v>72</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>98</v>
@@ -2773,7 +2945,7 @@
         <v>63</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>99</v>
@@ -2791,7 +2963,7 @@
         <v>21</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F88" s="3"/>
       <c r="H88" t="str">
@@ -2804,7 +2976,7 @@
         <v>66</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>101</v>
@@ -2823,7 +2995,7 @@
         <v>67</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>102</v>
@@ -2842,7 +3014,7 @@
         <v>68</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>103</v>
@@ -2895,7 +3067,7 @@
         <v>105</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>104</v>
@@ -2914,7 +3086,7 @@
         <v>109</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>108</v>
@@ -2942,7 +3114,7 @@
         <v>22</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>137</v>
@@ -2960,7 +3132,7 @@
         <v>91</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>90</v>
@@ -2978,7 +3150,7 @@
         <v>56</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>138</v>
@@ -2996,7 +3168,7 @@
         <v>23</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>89</v>
@@ -3023,7 +3195,7 @@
         <v>148</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>146</v>
@@ -3050,7 +3222,7 @@
         <v>152</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>150</v>
@@ -3065,7 +3237,7 @@
     </row>
     <row r="105" spans="1:8">
       <c r="H105" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fwr: update help anchors
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@81683 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -756,9 +756,6 @@
     <t>addingcaptionstoanen.htm</t>
   </si>
   <si>
-    <t>legacy dz</t>
-  </si>
-  <si>
     <t>uploadamediafileands.htm</t>
   </si>
   <si>
@@ -912,15 +909,9 @@
     <t>entriestab.htm</t>
   </si>
   <si>
-    <t>dz could not access - after creating clip</t>
-  </si>
-  <si>
     <t>replacingmedia.htm</t>
   </si>
   <si>
-    <t>dz could not create - ls still provistioning</t>
-  </si>
-  <si>
     <t>userstab.htm</t>
   </si>
   <si>
@@ -954,9 +945,6 @@
     <t>addvideoaudio.htm</t>
   </si>
   <si>
-    <t>dz- could not create</t>
-  </si>
-  <si>
     <t>themoderatationtab.htm</t>
   </si>
   <si>
@@ -1006,6 +994,18 @@
   </si>
   <si>
     <t>&lt;help&gt;</t>
+  </si>
+  <si>
+    <t>clippingandtrimmingm.htm</t>
+  </si>
+  <si>
+    <t>themixestab</t>
+  </si>
+  <si>
+    <t>configuringthelivest.htm</t>
+  </si>
+  <si>
+    <t>linktoremotestorage.htm</t>
   </si>
 </sst>
 </file>
@@ -1451,13 +1451,13 @@
   <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" style="5" customWidth="1"/>
     <col min="3" max="3" width="44.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="7" customWidth="1"/>
   </cols>
@@ -1481,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1489,7 +1489,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>74</v>
@@ -1576,7 +1576,7 @@
         <v>184</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>170</v>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_clips" anchor="dz could not access - after creating clip" /&gt;</v>
+        <v>&lt;item key="entry_clips" anchor="clippingandtrimmingm.htm" /&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1594,7 +1594,7 @@
         <v>185</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>246</v>
+        <v>327</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>171</v>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_content" anchor="legacy dz" /&gt;</v>
+        <v>&lt;item key="entry_content" anchor="themixestab" /&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1612,7 +1612,7 @@
         <v>186</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>172</v>
@@ -1630,7 +1630,7 @@
         <v>187</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>173</v>
@@ -1648,7 +1648,7 @@
         <v>188</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>174</v>
@@ -1666,7 +1666,7 @@
         <v>176</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>175</v>
@@ -1684,7 +1684,7 @@
         <v>188</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>85</v>
@@ -1694,7 +1694,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_live_stream" anchor="dz could not create - ls still provistioning" /&gt;</v>
+        <v>&lt;item key="section_live_stream" anchor="configuringthelivest.htm" /&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1702,7 +1702,7 @@
         <v>189</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>177</v>
@@ -1720,7 +1720,7 @@
         <v>190</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>178</v>
@@ -1738,7 +1738,7 @@
         <v>191</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>179</v>
@@ -1756,7 +1756,7 @@
         <v>192</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>180</v>
@@ -1774,7 +1774,7 @@
         <v>193</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>117</v>
@@ -1793,7 +1793,7 @@
         <v>194</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>114</v>
@@ -1811,7 +1811,7 @@
         <v>195</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>118</v>
@@ -1829,7 +1829,7 @@
         <v>196</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>120</v>
@@ -1847,7 +1847,7 @@
         <v>197</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>121</v>
@@ -1865,7 +1865,7 @@
         <v>221</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>220</v>
@@ -1883,7 +1883,7 @@
         <v>225</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>223</v>
@@ -1901,7 +1901,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>113</v>
@@ -1919,7 +1919,7 @@
         <v>157</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>155</v>
@@ -1937,7 +1937,7 @@
         <v>161</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>158</v>
@@ -1955,7 +1955,7 @@
         <v>163</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>159</v>
@@ -1973,7 +1973,7 @@
         <v>162</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>160</v>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_link" anchor="dz- could not create" /&gt;</v>
+        <v>&lt;item key="section_flavor_link" anchor="linktoremotestorage.htm" /&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1991,7 +1991,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>75</v>
@@ -2009,7 +2009,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>76</v>
@@ -2027,7 +2027,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>83</v>
@@ -2045,7 +2045,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>119</v>
@@ -2063,7 +2063,7 @@
         <v>24</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>112</v>
@@ -2081,7 +2081,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>77</v>
@@ -2096,10 +2096,10 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
+        <v>257</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>259</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>111</v>
@@ -2117,7 +2117,7 @@
         <v>11</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>110</v>
@@ -2135,7 +2135,7 @@
         <v>166</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>165</v>
@@ -2153,7 +2153,7 @@
         <v>199</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>198</v>
@@ -2171,7 +2171,7 @@
         <v>200</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>205</v>
@@ -2189,7 +2189,7 @@
         <v>201</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>204</v>
@@ -2207,7 +2207,7 @@
         <v>202</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>206</v>
@@ -2225,7 +2225,7 @@
         <v>207</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>209</v>
@@ -2243,7 +2243,7 @@
         <v>212</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>210</v>
@@ -2261,7 +2261,7 @@
         <v>215</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>214</v>
@@ -2279,7 +2279,7 @@
         <v>217</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>216</v>
@@ -2297,7 +2297,7 @@
         <v>219</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>218</v>
@@ -2315,7 +2315,7 @@
         <v>228</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>226</v>
@@ -2333,7 +2333,7 @@
         <v>235</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>229</v>
@@ -2351,7 +2351,7 @@
         <v>236</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>231</v>
@@ -2369,7 +2369,7 @@
         <v>237</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>233</v>
@@ -2407,7 +2407,7 @@
         <v>6</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>78</v>
@@ -2425,7 +2425,7 @@
         <v>79</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>80</v>
@@ -2443,7 +2443,7 @@
         <v>82</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>81</v>
@@ -2470,7 +2470,7 @@
         <v>13</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>122</v>
@@ -2488,7 +2488,7 @@
         <v>124</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>123</v>
@@ -2515,7 +2515,7 @@
         <v>15</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>125</v>
@@ -2533,7 +2533,7 @@
         <v>17</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>126</v>
@@ -2569,7 +2569,7 @@
         <v>240</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>238</v>
@@ -2587,7 +2587,7 @@
         <v>16</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>127</v>
@@ -2623,7 +2623,7 @@
         <v>129</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>128</v>
@@ -2641,7 +2641,7 @@
         <v>130</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>131</v>
@@ -2659,7 +2659,7 @@
         <v>142</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>143</v>
@@ -2677,7 +2677,7 @@
         <v>141</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>139</v>
@@ -2695,7 +2695,7 @@
         <v>48</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>132</v>
@@ -2713,7 +2713,7 @@
         <v>144</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="8" t="s">
@@ -2729,7 +2729,7 @@
         <v>87</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>86</v>
@@ -2747,7 +2747,7 @@
         <v>43</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>133</v>
@@ -2765,7 +2765,7 @@
         <v>135</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>134</v>
@@ -2792,7 +2792,7 @@
         <v>20</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>100</v>
@@ -2819,7 +2819,7 @@
         <v>57</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>92</v>
@@ -2837,7 +2837,7 @@
         <v>58</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>93</v>
@@ -2855,7 +2855,7 @@
         <v>59</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>94</v>
@@ -2873,7 +2873,7 @@
         <v>60</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>95</v>
@@ -2891,7 +2891,7 @@
         <v>61</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>96</v>
@@ -2909,7 +2909,7 @@
         <v>62</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>97</v>
@@ -2927,7 +2927,7 @@
         <v>72</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>98</v>
@@ -2945,7 +2945,7 @@
         <v>63</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>99</v>
@@ -2963,7 +2963,7 @@
         <v>21</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F88" s="3"/>
       <c r="H88" t="str">
@@ -2976,7 +2976,7 @@
         <v>66</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>101</v>
@@ -2995,7 +2995,7 @@
         <v>67</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>102</v>
@@ -3014,7 +3014,7 @@
         <v>68</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>103</v>
@@ -3067,7 +3067,7 @@
         <v>105</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>104</v>
@@ -3086,7 +3086,7 @@
         <v>109</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>108</v>
@@ -3114,7 +3114,7 @@
         <v>22</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>137</v>
@@ -3132,7 +3132,7 @@
         <v>91</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>90</v>
@@ -3150,7 +3150,7 @@
         <v>56</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>138</v>
@@ -3168,7 +3168,7 @@
         <v>23</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>89</v>
@@ -3195,7 +3195,7 @@
         <v>148</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>146</v>
@@ -3222,7 +3222,7 @@
         <v>152</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>150</v>
@@ -3237,7 +3237,7 @@
     </row>
     <row r="105" spans="1:8">
       <c r="H105" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
qnd: updates to help anchors
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@82702 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20775" windowHeight="13410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="339">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -741,271 +741,298 @@
     <t>edit category entitlement</t>
   </si>
   <si>
+    <t>editentrymenus.htm</t>
+  </si>
+  <si>
+    <t>creatinganaccessprof.htm</t>
+  </si>
+  <si>
+    <t>addingamidroll.htm</t>
+  </si>
+  <si>
+    <t>addingcaptionstoanen.htm</t>
+  </si>
+  <si>
+    <t>uploadamediafileands.htm</t>
+  </si>
+  <si>
+    <t>addingadistributorto.htm</t>
+  </si>
+  <si>
+    <t>theflavorstab.htm</t>
+  </si>
+  <si>
+    <t>uploadingandmodifyin.htm</t>
+  </si>
+  <si>
+    <t>contentscheduling.htm</t>
+  </si>
+  <si>
+    <t>troubleshootingtrimm.htm</t>
+  </si>
+  <si>
+    <t>uploadfromdesktop.htm</t>
+  </si>
+  <si>
+    <t>whatisaplaylist.htm</t>
+  </si>
+  <si>
+    <t>creatingamanualplayl.htm</t>
+  </si>
+  <si>
+    <t>creatingarulebasedpl.htm</t>
+  </si>
+  <si>
+    <t>definingarule.htm</t>
+  </si>
+  <si>
+    <t>add syndication field dz - note for google only</t>
+  </si>
+  <si>
+    <t>settingupsyndication.htm</t>
+  </si>
+  <si>
+    <t>kmcpublishertasksfor.htm</t>
+  </si>
+  <si>
+    <t>addacategory.htm</t>
+  </si>
+  <si>
+    <t>addingmetadatatoacat.htm</t>
+  </si>
+  <si>
+    <t>playerlist.htm</t>
+  </si>
+  <si>
+    <t>editingaplayer.htm</t>
+  </si>
+  <si>
+    <t>accountsettings.htm</t>
+  </si>
+  <si>
+    <t>integrationsettings.htm</t>
+  </si>
+  <si>
+    <t>convertingvideosinto.htm</t>
+  </si>
+  <si>
+    <t>addingatranscodingpr.htm</t>
+  </si>
+  <si>
+    <t>editingandcreatingtr.htm</t>
+  </si>
+  <si>
+    <t>Adding_Custom_Metadata_Fields</t>
+  </si>
+  <si>
+    <t>kalturacustommetadat.htm</t>
+  </si>
+  <si>
+    <t>addingaschema.htm</t>
+  </si>
+  <si>
+    <t>myusersettings.htm</t>
+  </si>
+  <si>
+    <t>accountupgrade.htm</t>
+  </si>
+  <si>
+    <t>bandwidthusagereport.htm</t>
+  </si>
+  <si>
+    <t>topcontent.htm</t>
+  </si>
+  <si>
+    <t>contentdropoff.htm</t>
+  </si>
+  <si>
+    <t>contentinteractions.htm</t>
+  </si>
+  <si>
+    <t>contentcontributions.htm</t>
+  </si>
+  <si>
+    <t>individualtopcontent.htm</t>
+  </si>
+  <si>
+    <t>individualcontentdro.htm</t>
+  </si>
+  <si>
+    <t>individualcontentint.htm</t>
+  </si>
+  <si>
+    <t>individualcontentcon.htm</t>
+  </si>
+  <si>
+    <t>userandcommunityrepo.htm</t>
+  </si>
+  <si>
+    <t>topcontributors.htm</t>
+  </si>
+  <si>
+    <t>geographicdistributi.htm</t>
+  </si>
+  <si>
+    <t>topsyndications.htm</t>
+  </si>
+  <si>
+    <t>userengagementreport.htm</t>
+  </si>
+  <si>
+    <t>individualuserengage.htm</t>
+  </si>
+  <si>
+    <t>purchasingalicensefo.htm</t>
+  </si>
+  <si>
+    <t>addingauser.htm</t>
+  </si>
+  <si>
+    <t>rolemanagement.htm</t>
+  </si>
+  <si>
+    <t>creatingcustomroles.htm</t>
+  </si>
+  <si>
+    <t>theuploadtab.htm</t>
+  </si>
+  <si>
+    <t>&lt;/help&gt;</t>
+  </si>
+  <si>
+    <t>entriestab.htm</t>
+  </si>
+  <si>
+    <t>replacingmedia.htm</t>
+  </si>
+  <si>
+    <t>userstab.htm</t>
+  </si>
+  <si>
+    <t>downloadfiles.htm</t>
+  </si>
+  <si>
+    <t>addtags1.htm</t>
+  </si>
+  <si>
+    <t>removingtags.htm</t>
+  </si>
+  <si>
+    <t>setaccesscontrol.htm</t>
+  </si>
+  <si>
+    <t>setscheduling.htm</t>
+  </si>
+  <si>
+    <t>changeowner1.htm</t>
+  </si>
+  <si>
+    <t>removecategories.htm</t>
+  </si>
+  <si>
+    <t>creatingalivestreami.htm</t>
+  </si>
+  <si>
+    <t>matchfilesfromdropfo.htm</t>
+  </si>
+  <si>
+    <t>addvideoaudio.htm</t>
+  </si>
+  <si>
+    <t>themoderatationtab.htm</t>
+  </si>
+  <si>
+    <t>thecategoriestab.htm</t>
+  </si>
+  <si>
+    <t>subcategories.htm</t>
+  </si>
+  <si>
+    <t>enduseraccesspermiss.htm</t>
+  </si>
+  <si>
+    <t>addinguserpermission.htm</t>
+  </si>
+  <si>
+    <t>addtags.htm</t>
+  </si>
+  <si>
+    <t>removetags.htm</t>
+  </si>
+  <si>
+    <t>movecategories.htm</t>
+  </si>
+  <si>
+    <t>changelisting.htm</t>
+  </si>
+  <si>
+    <t>changeaccess.htm</t>
+  </si>
+  <si>
+    <t>changeowner.htm</t>
+  </si>
+  <si>
+    <t>youruploads.htm</t>
+  </si>
+  <si>
+    <t>bulkuploadlog.htm</t>
+  </si>
+  <si>
+    <t>usingadropfolder.htm</t>
+  </si>
+  <si>
+    <t>addingentitlementcon.htm</t>
+  </si>
+  <si>
+    <t>&lt;help&gt;</t>
+  </si>
+  <si>
+    <t>clippingandtrimmingm.htm</t>
+  </si>
+  <si>
+    <t>configuringthelivest.htm</t>
+  </si>
+  <si>
+    <t>linktoremotestorage.htm</t>
+  </si>
+  <si>
+    <t>categoryenduserentit.htm</t>
+  </si>
+  <si>
+    <t>accesscontrolprofile.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content Privacy </t>
+  </si>
+  <si>
+    <t>addingorremovinggeog.htm</t>
+  </si>
+  <si>
+    <t>addingorremovingipad.htm</t>
+  </si>
+  <si>
+    <t>themixestab</t>
+  </si>
+  <si>
+    <t>add domain</t>
+  </si>
+  <si>
+    <t>add/remove countries</t>
+  </si>
+  <si>
+    <t>add/remove ip addresses</t>
+  </si>
+  <si>
+    <t>preview and embed</t>
+  </si>
+  <si>
+    <t>section_pne</t>
+  </si>
+  <si>
+    <t>html wrapper</t>
+  </si>
+  <si>
     <t>Nethelp - dz</t>
-  </si>
-  <si>
-    <t>editentrymenus.htm</t>
-  </si>
-  <si>
-    <t>creatinganaccessprof.htm</t>
-  </si>
-  <si>
-    <t>addingamidroll.htm</t>
-  </si>
-  <si>
-    <t>addingcaptionstoanen.htm</t>
-  </si>
-  <si>
-    <t>uploadamediafileands.htm</t>
-  </si>
-  <si>
-    <t>addingadistributorto.htm</t>
-  </si>
-  <si>
-    <t>theflavorstab.htm</t>
-  </si>
-  <si>
-    <t>uploadingandmodifyin.htm</t>
-  </si>
-  <si>
-    <t>contentscheduling.htm</t>
-  </si>
-  <si>
-    <t>troubleshootingtrimm.htm</t>
-  </si>
-  <si>
-    <t>uploadfromdesktop.htm</t>
-  </si>
-  <si>
-    <t>whatisaplaylist.htm</t>
-  </si>
-  <si>
-    <t>creatingamanualplayl.htm</t>
-  </si>
-  <si>
-    <t>creatingarulebasedpl.htm</t>
-  </si>
-  <si>
-    <t>definingarule.htm</t>
-  </si>
-  <si>
-    <t>add syndication field dz - note for google only</t>
-  </si>
-  <si>
-    <t>settingupsyndication.htm</t>
-  </si>
-  <si>
-    <t>kmcpublishertasksfor.htm</t>
-  </si>
-  <si>
-    <t>addacategory.htm</t>
-  </si>
-  <si>
-    <t>addingmetadatatoacat.htm</t>
-  </si>
-  <si>
-    <t>playerlist.htm</t>
-  </si>
-  <si>
-    <t>editingaplayer.htm</t>
-  </si>
-  <si>
-    <t>accountsettings.htm</t>
-  </si>
-  <si>
-    <t>integrationsettings.htm</t>
-  </si>
-  <si>
-    <t>contententitlement.htm</t>
-  </si>
-  <si>
-    <t>convertingvideosinto.htm</t>
-  </si>
-  <si>
-    <t>addingatranscodingpr.htm</t>
-  </si>
-  <si>
-    <t>editingandcreatingtr.htm</t>
-  </si>
-  <si>
-    <t>Adding_Custom_Metadata_Fields</t>
-  </si>
-  <si>
-    <t>kalturacustommetadat.htm</t>
-  </si>
-  <si>
-    <t>addingaschema.htm</t>
-  </si>
-  <si>
-    <t>myusersettings.htm</t>
-  </si>
-  <si>
-    <t>accountupgrade.htm</t>
-  </si>
-  <si>
-    <t>bandwidthusagereport.htm</t>
-  </si>
-  <si>
-    <t>topcontent.htm</t>
-  </si>
-  <si>
-    <t>contentdropoff.htm</t>
-  </si>
-  <si>
-    <t>contentinteractions.htm</t>
-  </si>
-  <si>
-    <t>contentcontributions.htm</t>
-  </si>
-  <si>
-    <t>individualtopcontent.htm</t>
-  </si>
-  <si>
-    <t>individualcontentdro.htm</t>
-  </si>
-  <si>
-    <t>individualcontentint.htm</t>
-  </si>
-  <si>
-    <t>individualcontentcon.htm</t>
-  </si>
-  <si>
-    <t>userandcommunityrepo.htm</t>
-  </si>
-  <si>
-    <t>topcontributors.htm</t>
-  </si>
-  <si>
-    <t>geographicdistributi.htm</t>
-  </si>
-  <si>
-    <t>topsyndications.htm</t>
-  </si>
-  <si>
-    <t>userengagementreport.htm</t>
-  </si>
-  <si>
-    <t>individualuserengage.htm</t>
-  </si>
-  <si>
-    <t>purchasingalicensefo.htm</t>
-  </si>
-  <si>
-    <t>addingauser.htm</t>
-  </si>
-  <si>
-    <t>rolemanagement.htm</t>
-  </si>
-  <si>
-    <t>creatingcustomroles.htm</t>
-  </si>
-  <si>
-    <t>theuploadtab.htm</t>
-  </si>
-  <si>
-    <t>&lt;/help&gt;</t>
-  </si>
-  <si>
-    <t>entriestab.htm</t>
-  </si>
-  <si>
-    <t>replacingmedia.htm</t>
-  </si>
-  <si>
-    <t>userstab.htm</t>
-  </si>
-  <si>
-    <t>downloadfiles.htm</t>
-  </si>
-  <si>
-    <t>addtags1.htm</t>
-  </si>
-  <si>
-    <t>removingtags.htm</t>
-  </si>
-  <si>
-    <t>setaccesscontrol.htm</t>
-  </si>
-  <si>
-    <t>setscheduling.htm</t>
-  </si>
-  <si>
-    <t>changeowner1.htm</t>
-  </si>
-  <si>
-    <t>removecategories.htm</t>
-  </si>
-  <si>
-    <t>creatingalivestreami.htm</t>
-  </si>
-  <si>
-    <t>matchfilesfromdropfo.htm</t>
-  </si>
-  <si>
-    <t>addvideoaudio.htm</t>
-  </si>
-  <si>
-    <t>themoderatationtab.htm</t>
-  </si>
-  <si>
-    <t>thecategoriestab.htm</t>
-  </si>
-  <si>
-    <t>categoryenduseracces.htm</t>
-  </si>
-  <si>
-    <t>subcategories.htm</t>
-  </si>
-  <si>
-    <t>enduseraccesspermiss.htm</t>
-  </si>
-  <si>
-    <t>addinguserpermission.htm</t>
-  </si>
-  <si>
-    <t>addtags.htm</t>
-  </si>
-  <si>
-    <t>removetags.htm</t>
-  </si>
-  <si>
-    <t>movecategories.htm</t>
-  </si>
-  <si>
-    <t>changelisting.htm</t>
-  </si>
-  <si>
-    <t>changeaccess.htm</t>
-  </si>
-  <si>
-    <t>changeowner.htm</t>
-  </si>
-  <si>
-    <t>youruploads.htm</t>
-  </si>
-  <si>
-    <t>bulkuploadlog.htm</t>
-  </si>
-  <si>
-    <t>usingadropfolder.htm</t>
-  </si>
-  <si>
-    <t>addingentitlementcon.htm</t>
-  </si>
-  <si>
-    <t>&lt;help&gt;</t>
-  </si>
-  <si>
-    <t>clippingandtrimmingm.htm</t>
-  </si>
-  <si>
-    <t>themixestab</t>
-  </si>
-  <si>
-    <t>configuringthelivest.htm</t>
-  </si>
-  <si>
-    <t>linktoremotestorage.htm</t>
   </si>
 </sst>
 </file>
@@ -1068,13 +1095,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1108,6 +1135,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1124,7 +1157,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1142,8 +1175,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1448,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1467,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>241</v>
+        <v>338</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>73</v>
@@ -1481,915 +1521,921 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>296</v>
-      </c>
+      <c r="A3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" s="14"/>
       <c r="C3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>336</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("&lt;item key=""",C3,""" anchor=""",B3,""" /&gt;")</f>
+        <v>&lt;item key="section_pne" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="str">
+        <f>CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
         <v>&lt;item key="section_entries" anchor="entriestab.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" ref="H4:H67" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
-        <v>&lt;item key="" anchor="editentrymenus.htm" /&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="entry_accesscontrol" anchor="creatinganaccessprof.htm" /&gt;</v>
+        <f t="shared" ref="H5:H67" si="0">CONCATENATE("&lt;item key=""",C5,""" anchor=""",B5,""" /&gt;")</f>
+        <v>&lt;item key="" anchor="editentrymenus.htm" /&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_ads" anchor="addingamidroll.htm" /&gt;</v>
+        <v>&lt;item key="entry_accesscontrol" anchor="creatinganaccessprof.htm" /&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_captions" anchor="addingcaptionstoanen.htm" /&gt;</v>
+        <v>&lt;item key="entry_ads" anchor="addingamidroll.htm" /&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>326</v>
+        <v>182</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>244</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_clips" anchor="clippingandtrimmingm.htm" /&gt;</v>
+        <v>&lt;item key="entry_captions" anchor="addingcaptionstoanen.htm" /&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>185</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>327</v>
+        <v>184</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>323</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_content" anchor="themixestab" /&gt;</v>
+        <v>&lt;item key="entry_clips" anchor="clippingandtrimmingm.htm" /&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>186</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>246</v>
+        <v>185</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>331</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_metadata" anchor="uploadamediafileands.htm" /&gt;</v>
+        <v>&lt;item key="entry_content" anchor="themixestab" /&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_distribution" anchor="addingadistributorto.htm" /&gt;</v>
+        <v>&lt;item key="entry_metadata" anchor="uploadamediafileands.htm" /&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_flavors" anchor="theflavorstab.htm" /&gt;</v>
+        <v>&lt;item key="entry_distribution" anchor="addingadistributorto.htm" /&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>297</v>
+        <v>247</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_replacement" anchor="replacingmedia.htm" /&gt;</v>
+        <v>&lt;item key="entry_flavors" anchor="theflavorstab.htm" /&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>328</v>
+        <v>176</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>295</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>85</v>
+        <v>175</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_live_stream" anchor="configuringthelivest.htm" /&gt;</v>
+        <v>&lt;item key="entry_replacement" anchor="replacingmedia.htm" /&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>249</v>
+        <v>324</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>177</v>
+        <v>85</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_related" anchor="uploadingandmodifyin.htm" /&gt;</v>
+        <v>&lt;item key="section_live_stream" anchor="configuringthelivest.htm" /&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_scheduling" anchor="contentscheduling.htm" /&gt;</v>
+        <v>&lt;item key="entry_related" anchor="uploadingandmodifyin.htm" /&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_thumbnails" anchor="troubleshootingtrimm.htm" /&gt;</v>
+        <v>&lt;item key="entry_scheduling" anchor="contentscheduling.htm" /&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>298</v>
+        <v>250</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_users" anchor="userstab.htm" /&gt;</v>
+        <v>&lt;item key="entry_thumbnails" anchor="troubleshootingtrimm.htm" /&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>37</v>
+      </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_download" anchor="downloadfiles.htm" /&gt;</v>
+        <v>&lt;item key="entry_users" anchor="userstab.htm" /&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>115</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F20" s="3"/>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_entry_tags" anchor="addtags1.htm" /&gt;</v>
+        <v>&lt;item key="section_download" anchor="downloadfiles.htm" /&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_remove_entry_tags" anchor="removingtags.htm" /&gt;</v>
+        <v>&lt;item key="section_add_entry_tags" anchor="addtags1.htm" /&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_access_control" anchor="setaccesscontrol.htm" /&gt;</v>
+        <v>&lt;item key="section_remove_entry_tags" anchor="removingtags.htm" /&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_sched" anchor="setscheduling.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_access_control" anchor="setaccesscontrol.htm" /&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>220</v>
+        <v>121</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>222</v>
+        <v>52</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entry_owner" anchor="changeowner1.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_sched" anchor="setscheduling.htm" /&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entry_remove_cats" anchor="removecategories.htm" /&gt;</v>
+        <v>&lt;item key="section_entry_owner" anchor="changeowner1.htm" /&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>306</v>
+        <v>225</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>303</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>113</v>
+        <v>223</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>33</v>
+        <v>224</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_live_stream" anchor="creatingalivestreami.htm" /&gt;</v>
+        <v>&lt;item key="section_entry_remove_cats" anchor="removecategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_dropfolder" anchor="matchfilesfromdropfo.htm" /&gt;</v>
+        <v>&lt;item key="section_add_live_stream" anchor="creatingalivestreami.htm" /&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>252</v>
+        <v>305</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_upload" anchor="uploadfromdesktop.htm" /&gt;</v>
+        <v>&lt;item key="section_flavor_dropfolder" anchor="matchfilesfromdropfo.htm" /&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>308</v>
+        <v>251</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>164</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_import" anchor="addvideoaudio.htm" /&gt;</v>
+        <v>&lt;item key="section_flavor_upload" anchor="uploadfromdesktop.htm" /&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>162</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>329</v>
+        <v>163</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>306</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>164</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
+        <v>&lt;item key="section_flavor_import" anchor="addvideoaudio.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_flavor_link" anchor="linktoremotestorage.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_moderation" anchor="themoderatationtab.htm" /&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>253</v>
+        <v>307</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
+        <v>&lt;item key="section_moderation" anchor="themoderatationtab.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_playlists" anchor="whatisaplaylist.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H33" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_manual_playlist" anchor="creatingamanualplayl.htm" /&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H34" t="str">
-        <f>CONCATENATE("&lt;item key=""",C34,""" anchor=""",B34,""" /&gt;")</f>
-        <v>&lt;item key="section_rule_playlist" anchor="creatingarulebasedpl.htm" /&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_manual_playlist" anchor="creatingamanualplayl.htm" /&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" t="str">
+        <f>CONCATENATE("&lt;item key=""",C35,""" anchor=""",B35,""" /&gt;")</f>
+        <v>&lt;item key="section_rule_playlist" anchor="creatingarulebasedpl.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="B36" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H35" t="str">
+      <c r="H36" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_edit_rule" anchor="definingarule.htm" /&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="B37" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H36" t="str">
+      <c r="H37" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_syndication" anchor="settingupsyndication.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>257</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H37" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_ExternalSyndicationPopup" anchor="settingupsyndication.htm" /&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
+        <v>256</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_ExternalSyndicationPopup" anchor="settingupsyndication.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="B39" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H38" t="str">
+      <c r="H39" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_ExternalSyndicationNotification" anchor="kmcpublishertasksfor.htm" /&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="B40" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H39" t="str">
+      <c r="H40" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_categories" anchor="thecategoriestab.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="H40" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_parent" anchor="addacategory.htm" /&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>203</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
+        <v>&lt;item key="section_category_parent" anchor="addacategory.htm" /&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>311</v>
+        <v>260</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>203</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_users" anchor="categoryenduseracces.htm" /&gt;</v>
+        <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>312</v>
+        <v>201</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>326</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>203</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_subcats" anchor="subcategories.htm" /&gt;</v>
+        <v>&lt;item key="section_category_users" anchor="categoryenduserentit.htm" /&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_permission" anchor="enduseraccesspermiss.htm" /&gt;</v>
+        <v>&lt;item key="section_category_subcats" anchor="subcategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>210</v>
+        <v>310</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_add" anchor="addacategory.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_user_permission" anchor="enduseraccesspermiss.htm" /&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>314</v>
+        <v>259</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_user_add" anchor="addacategory.htm" /&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
+        <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>227</v>
+        <v>116</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
+        <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_list" anchor="changelisting.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_access" anchor="changeaccess.htm" /&gt;</v>
+        <v>&lt;item key="section_cats_list" anchor="changelisting.htm" /&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_cats_access" anchor="changeaccess.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="C52" s="6" t="s">
+      <c r="B53" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D53" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="H52" t="str">
+      <c r="H53" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_cats_owner" anchor="changeowner.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="4"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="8"/>
-      <c r="H53" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2407,7 +2453,7 @@
         <v>6</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>78</v>
@@ -2425,7 +2471,7 @@
         <v>79</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>80</v>
@@ -2443,7 +2489,7 @@
         <v>82</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>81</v>
@@ -2470,7 +2516,7 @@
         <v>13</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>122</v>
@@ -2488,7 +2534,7 @@
         <v>124</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>123</v>
@@ -2515,7 +2561,7 @@
         <v>15</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>125</v>
@@ -2533,7 +2579,7 @@
         <v>17</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>126</v>
@@ -2569,7 +2615,7 @@
         <v>240</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>238</v>
@@ -2586,8 +2632,8 @@
       <c r="A66" t="s">
         <v>16</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>266</v>
+      <c r="B66" s="12" t="s">
+        <v>327</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>127</v>
@@ -2597,15 +2643,15 @@
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_acc_access_control" anchor="contententitlement.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_access_control" anchor="accesscontrolprofile.htm" /&gt;</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>18</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>243</v>
+      <c r="B67" s="14" t="s">
+        <v>328</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>84</v>
@@ -2615,426 +2661,413 @@
       </c>
       <c r="H67" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_access_control_profile" anchor="creatinganaccessprof.htm" /&gt;</v>
+        <v>&lt;item key="section_access_control_profile" anchor="Content Privacy " /&gt;</v>
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" t="s">
-        <v>129</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="A68" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="D68" s="8"/>
       <c r="H68" t="str">
         <f t="shared" ref="H68:H85" si="1">CONCATENATE("&lt;item key=""",C68,""" anchor=""",B68,""" /&gt;")</f>
-        <v>&lt;item key="section_acc_transcoding_def" anchor="convertingvideosinto.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="Content Privacy " /&gt;</v>
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" t="s">
-        <v>130</v>
+      <c r="A69" s="13" t="s">
+        <v>333</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>44</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="D69" s="8"/>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_acc_transcoding_profiles" anchor="addingatranscodingpr.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="addingorremovinggeog.htm" /&gt;</v>
       </c>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" t="s">
-        <v>142</v>
+      <c r="A70" s="13" t="s">
+        <v>334</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>50</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="D70" s="8"/>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_transcoding_profile_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="addingorremovingipad.htm" /&gt;</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>140</v>
+        <v>44</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_transcoding_flavor_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_transcoding_def" anchor="convertingvideosinto.htm" /&gt;</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>48</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_acc_custom_data" anchor="Adding_Custom_Metadata_Fields" /&gt;</v>
+        <v>&lt;item key="section_acc_transcoding_profiles" anchor="addingatranscodingpr.htm" /&gt;</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>144</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="C73" s="6"/>
+        <v>142</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="D73" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="kalturacustommetadat.htm" /&gt;</v>
+        <v>&lt;item key="section_transcoding_profile_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>87</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>86</v>
+        <v>141</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_custom_data_field" anchor="addingaschema.htm" /&gt;</v>
+        <v>&lt;item key="section_transcoding_flavor_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>43</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>133</v>
+        <v>48</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_acc_user" anchor="myusersettings.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_custom_data" anchor="Adding_Custom_Metadata_Fields" /&gt;</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>135</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>134</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C76" s="6"/>
       <c r="D76" s="8" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_acc_upgrade" anchor="accountupgrade.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="18.75">
-      <c r="A77" s="2" t="s">
-        <v>19</v>
+        <v>&lt;item key="" anchor="kalturacustommetadat.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
+        <v>&lt;item key="section_custom_data_field" anchor="addingaschema.htm" /&gt;</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>20</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>100</v>
+        <v>43</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_analytics_usage" anchor="bandwidthusagereport.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_user" anchor="myusersettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="1" t="s">
-        <v>64</v>
+      <c r="A79" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>39</v>
+        <v>&lt;item key="section_acc_upgrade" anchor="accountupgrade.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="18.75">
+      <c r="A80" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_analytics_top_content" anchor="topcontent.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_analytics_content_dropoff" anchor="contentdropoff.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_usage" anchor="bandwidthusagereport.htm" /&gt;</v>
       </c>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" t="s">
-        <v>59</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>39</v>
+      <c r="A82" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_analytics_content_interactions" anchor="contentinteractions.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" t="s">
-        <v>60</v>
+      <c r="A83" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_analytics_content_contribution" anchor="contentcontributions.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_content" anchor="topcontent.htm" /&gt;</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_analytics_video_drilldown" anchor="individualtopcontent.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_content_dropoff" anchor="contentdropoff.htm" /&gt;</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="individualcontentdro.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_content_interactions" anchor="contentinteractions.htm" /&gt;</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H86" t="str">
         <f>CONCATENATE("&lt;item key=""",C86,""" anchor=""",B86,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="individualcontentint.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_content_contribution" anchor="contentcontributions.htm" /&gt;</v>
       </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H87" t="str">
-        <f t="shared" ref="H87:H104" si="2">CONCATENATE("&lt;item key=""",C87,""" anchor=""",B87,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="individualcontentcon.htm" /&gt;</v>
+        <f t="shared" ref="H87:H107" si="2">CONCATENATE("&lt;item key=""",C87,""" anchor=""",B87,""" /&gt;")</f>
+        <v>&lt;item key="section_analytics_video_drilldown" anchor="individualtopcontent.htm" /&gt;</v>
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>284</v>
+      <c r="A88" t="s">
+        <v>62</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="F88" s="3"/>
       <c r="H88" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="userandcommunityrepo.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="individualcontentdro.htm" /&gt;</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="F89" s="3"/>
       <c r="H89" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributors.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="individualcontentint.htm" /&gt;</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="F90" s="3"/>
       <c r="H90" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="individualcontentcon.htm" /&gt;</v>
       </c>
     </row>
     <row r="91" spans="1:8">
-      <c r="A91" t="s">
-        <v>68</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>65</v>
+      <c r="A91" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>282</v>
       </c>
       <c r="F91" s="3"/>
       <c r="H91" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="userandcommunityrepo.htm" /&gt;</v>
       </c>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>69</v>
-      </c>
-      <c r="B92" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="C92" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>65</v>
@@ -3042,16 +3075,18 @@
       <c r="F92" s="3"/>
       <c r="H92" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributors.htm" /&gt;</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>70</v>
-      </c>
-      <c r="B93" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>284</v>
+      </c>
       <c r="C93" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>65</v>
@@ -3059,18 +3094,18 @@
       <c r="F93" s="3"/>
       <c r="H93" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_map_drilldown" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>65</v>
@@ -3078,18 +3113,16 @@
       <c r="F94" s="3"/>
       <c r="H94" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>109</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>289</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B95" s="6"/>
       <c r="C95" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>65</v>
@@ -3097,147 +3130,199 @@
       <c r="F95" s="3"/>
       <c r="H95" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_user_drilldown" anchor="individualuserengage.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="18.75">
-      <c r="A96" s="2" t="s">
-        <v>71</v>
+        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>70</v>
+      </c>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_drilldown" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>22</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D97" s="10" t="s">
-        <v>55</v>
+        <v>105</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_admin_users" anchor="purchasingalicensefo.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>91</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>90</v>
+        <v>109</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
-      <c r="A99" t="s">
-        <v>56</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D99" s="10" t="s">
-        <v>54</v>
+        <v>&lt;item key="section_analytics_user_drilldown" anchor="individualuserengage.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="18.75">
+      <c r="A99" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>41</v>
+        <v>137</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_role_drilldown" anchor="creatingcustomroles.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="18.75">
-      <c r="A101" s="2" t="s">
-        <v>145</v>
+        <v>&lt;item key="section_admin_users" anchor="purchasingalicensefo.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>91</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
+        <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>147</v>
+        <v>138</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_desktop_upload" anchor="theuploadtab.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="18.75">
-      <c r="A103" s="2" t="s">
-        <v>149</v>
+        <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>23</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
-      <c r="A104" t="s">
-        <v>152</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>151</v>
+        <v>&lt;item key="section_role_drilldown" anchor="creatingcustomroles.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="18.75">
+      <c r="A104" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="2"/>
+        <v>&lt;item key="" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>148</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H105" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;item key="section_desktop_upload" anchor="theuploadtab.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="18.75">
+      <c r="A106" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H106" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;item key="" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>152</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H107" t="str">
+        <f t="shared" si="2"/>
         <v>&lt;item key="section_upload_menu" anchor="theuploadtab.htm" /&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
-      <c r="H105" t="s">
-        <v>295</v>
+    <row r="108" spans="1:8">
+      <c r="H108" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
qnd: help links update
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@82778 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10920"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20520" windowHeight="10860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="347">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -822,9 +822,6 @@
     <t>editingandcreatingtr.htm</t>
   </si>
   <si>
-    <t>Adding_Custom_Metadata_Fields</t>
-  </si>
-  <si>
     <t>kalturacustommetadat.htm</t>
   </si>
   <si>
@@ -1002,18 +999,12 @@
     <t>accesscontrolprofile.htm</t>
   </si>
   <si>
-    <t xml:space="preserve">Content Privacy </t>
-  </si>
-  <si>
     <t>addingorremovinggeog.htm</t>
   </si>
   <si>
     <t>addingorremovingipad.htm</t>
   </si>
   <si>
-    <t>themixestab</t>
-  </si>
-  <si>
     <t>add domain</t>
   </si>
   <si>
@@ -1045,6 +1036,27 @@
   </si>
   <si>
     <t>section_pne_stream</t>
+  </si>
+  <si>
+    <t>embeddingaplayerwith.htm</t>
+  </si>
+  <si>
+    <t>mobilesupport.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">videodeliverysetting.htm </t>
+  </si>
+  <si>
+    <t>themixestab dz - legacy no? how do I get this tab</t>
+  </si>
+  <si>
+    <t>editinganaccessprof.htm</t>
+  </si>
+  <si>
+    <t>addingorremovingadom.htm</t>
+  </si>
+  <si>
+    <t>managingschemas.htm</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1181,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1196,6 +1208,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1500,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1519,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>73</v>
@@ -1533,55 +1548,61 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>335</v>
-      </c>
-      <c r="B3" s="14"/>
+        <v>332</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>340</v>
+      </c>
       <c r="C3" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("&lt;item key=""",C3,""" anchor=""",B3,""" /&gt;")</f>
-        <v>&lt;item key="section_pne" anchor="" /&gt;</v>
+        <v>&lt;item key="section_pne" anchor="embeddingaplayerwith.htm" /&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>339</v>
-      </c>
-      <c r="B4" s="14"/>
+        <v>336</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>341</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" ref="H4:H5" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
-        <v>&lt;item key="section_pne_ipad" anchor="" /&gt;</v>
+        <v>&lt;item key="section_pne_ipad" anchor="mobilesupport.htm" /&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>340</v>
-      </c>
-      <c r="B5" s="14"/>
+        <v>337</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>342</v>
+      </c>
       <c r="C5" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_pne_stream" anchor="" /&gt;</v>
+        <v>&lt;item key="section_pne_stream" anchor="videodeliverysetting.htm " /&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1589,7 +1610,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>74</v>
@@ -1676,7 +1697,7 @@
         <v>184</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>170</v>
@@ -1694,7 +1715,7 @@
         <v>185</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>171</v>
@@ -1704,7 +1725,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="entry_content" anchor="themixestab" /&gt;</v>
+        <v>&lt;item key="entry_content" anchor="themixestab dz - legacy no? how do I get this tab" /&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1766,7 +1787,7 @@
         <v>176</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>175</v>
@@ -1784,7 +1805,7 @@
         <v>188</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>85</v>
@@ -1856,7 +1877,7 @@
         <v>192</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>180</v>
@@ -1874,7 +1895,7 @@
         <v>193</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>117</v>
@@ -1893,7 +1914,7 @@
         <v>194</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>114</v>
@@ -1911,7 +1932,7 @@
         <v>195</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>118</v>
@@ -1929,7 +1950,7 @@
         <v>196</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>120</v>
@@ -1947,7 +1968,7 @@
         <v>197</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>121</v>
@@ -1965,7 +1986,7 @@
         <v>221</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>220</v>
@@ -1983,7 +2004,7 @@
         <v>225</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>223</v>
@@ -2001,7 +2022,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>113</v>
@@ -2019,7 +2040,7 @@
         <v>157</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>155</v>
@@ -2055,7 +2076,7 @@
         <v>163</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>159</v>
@@ -2073,7 +2094,7 @@
         <v>162</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>160</v>
@@ -2091,7 +2112,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>75</v>
@@ -2235,7 +2256,7 @@
         <v>166</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>165</v>
@@ -2289,7 +2310,7 @@
         <v>201</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>204</v>
@@ -2307,7 +2328,7 @@
         <v>202</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>206</v>
@@ -2325,7 +2346,7 @@
         <v>207</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>209</v>
@@ -2361,7 +2382,7 @@
         <v>215</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>214</v>
@@ -2379,7 +2400,7 @@
         <v>217</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>216</v>
@@ -2397,7 +2418,7 @@
         <v>219</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>218</v>
@@ -2415,7 +2436,7 @@
         <v>228</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>226</v>
@@ -2433,7 +2454,7 @@
         <v>235</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>229</v>
@@ -2451,7 +2472,7 @@
         <v>236</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>231</v>
@@ -2469,7 +2490,7 @@
         <v>237</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>233</v>
@@ -2497,7 +2518,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>78</v>
@@ -2515,7 +2536,7 @@
         <v>79</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>80</v>
@@ -2533,7 +2554,7 @@
         <v>82</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>81</v>
@@ -2659,7 +2680,7 @@
         <v>240</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>238</v>
@@ -2677,7 +2698,7 @@
         <v>16</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>127</v>
@@ -2694,8 +2715,8 @@
       <c r="A69" t="s">
         <v>18</v>
       </c>
-      <c r="B69" s="14" t="s">
-        <v>328</v>
+      <c r="B69" s="16" t="s">
+        <v>242</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>84</v>
@@ -2705,46 +2726,46 @@
       </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_access_control_profile" anchor="Content Privacy " /&gt;</v>
+        <v>&lt;item key="section_access_control_profile" anchor="creatinganaccessprof.htm" /&gt;</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="13" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="D70" s="8"/>
       <c r="H70" t="str">
         <f t="shared" ref="H70:H87" si="2">CONCATENATE("&lt;item key=""",C70,""" anchor=""",B70,""" /&gt;")</f>
-        <v>&lt;item key="" anchor="Content Privacy " /&gt;</v>
+        <v>&lt;item key="" anchor="editinganaccessprof.htm" /&gt;</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>345</v>
       </c>
       <c r="D71" s="8"/>
       <c r="H71" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="addingorremovinggeog.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="addingorremovingadom.htm" /&gt;</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="13" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D72" s="8"/>
       <c r="H72" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="addingorremovingipad.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="addingorremovinggeog.htm" /&gt;</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2752,7 +2773,7 @@
         <v>129</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>265</v>
+        <v>328</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>128</v>
@@ -2762,7 +2783,7 @@
       </c>
       <c r="H73" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_transcoding_def" anchor="convertingvideosinto.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_transcoding_def" anchor="addingorremovingipad.htm" /&gt;</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2770,7 +2791,7 @@
         <v>130</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>131</v>
@@ -2780,7 +2801,7 @@
       </c>
       <c r="H74" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_transcoding_profiles" anchor="addingatranscodingpr.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_transcoding_profiles" anchor="convertingvideosinto.htm" /&gt;</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2788,7 +2809,7 @@
         <v>142</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>143</v>
@@ -2798,7 +2819,7 @@
       </c>
       <c r="H75" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_transcoding_profile_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
+        <v>&lt;item key="section_transcoding_profile_edit" anchor="addingatranscodingpr.htm" /&gt;</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2823,8 +2844,8 @@
       <c r="A77" t="s">
         <v>48</v>
       </c>
-      <c r="B77" s="15" t="s">
-        <v>268</v>
+      <c r="B77" s="5" t="s">
+        <v>267</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>132</v>
@@ -2834,15 +2855,15 @@
       </c>
       <c r="H77" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_custom_data" anchor="Adding_Custom_Metadata_Fields" /&gt;</v>
+        <v>&lt;item key="section_acc_custom_data" anchor="editingandcreatingtr.htm" /&gt;</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>144</v>
       </c>
-      <c r="B78" s="6" t="s">
-        <v>269</v>
+      <c r="B78" s="15" t="s">
+        <v>346</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="8" t="s">
@@ -2850,15 +2871,15 @@
       </c>
       <c r="H78" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="kalturacustommetadat.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="managingschemas.htm" /&gt;</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>87</v>
       </c>
-      <c r="B79" s="6" t="s">
-        <v>270</v>
+      <c r="B79" s="15" t="s">
+        <v>269</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>86</v>
@@ -2875,8 +2896,8 @@
       <c r="A80" t="s">
         <v>43</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>271</v>
+      <c r="B80" s="6" t="s">
+        <v>268</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>133</v>
@@ -2886,15 +2907,15 @@
       </c>
       <c r="H80" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_user" anchor="myusersettings.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_user" anchor="kalturacustommetadat.htm" /&gt;</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>135</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>272</v>
+      <c r="B81" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>134</v>
@@ -2904,24 +2925,27 @@
       </c>
       <c r="H81" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_upgrade" anchor="accountupgrade.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_upgrade" anchor="addingaschema.htm" /&gt;</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="18.75">
       <c r="A82" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B82" s="5" t="s">
+        <v>270</v>
+      </c>
       <c r="H82" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
+        <v>&lt;item key="" anchor="myusersettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>20</v>
       </c>
-      <c r="B83" s="6" t="s">
-        <v>273</v>
+      <c r="B83" s="5" t="s">
+        <v>271</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>100</v>
@@ -2931,7 +2955,7 @@
       </c>
       <c r="H83" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_usage" anchor="bandwidthusagereport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_usage" anchor="accountupgrade.htm" /&gt;</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2948,7 +2972,7 @@
         <v>57</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>92</v>
@@ -2958,16 +2982,13 @@
       </c>
       <c r="H85" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_top_content" anchor="topcontent.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_content" anchor="bandwidthusagereport.htm" /&gt;</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>58</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>275</v>
-      </c>
       <c r="C86" s="6" t="s">
         <v>93</v>
       </c>
@@ -2976,7 +2997,7 @@
       </c>
       <c r="H86" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_content_dropoff" anchor="contentdropoff.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_content_dropoff" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2984,7 +3005,7 @@
         <v>59</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>94</v>
@@ -2994,7 +3015,7 @@
       </c>
       <c r="H87" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_content_interactions" anchor="contentinteractions.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_content_interactions" anchor="topcontent.htm" /&gt;</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -3002,7 +3023,7 @@
         <v>60</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>95</v>
@@ -3012,7 +3033,7 @@
       </c>
       <c r="H88" t="str">
         <f>CONCATENATE("&lt;item key=""",C88,""" anchor=""",B88,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_content_contribution" anchor="contentcontributions.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_content_contribution" anchor="contentdropoff.htm" /&gt;</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -3020,7 +3041,7 @@
         <v>61</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>96</v>
@@ -3030,7 +3051,7 @@
       </c>
       <c r="H89" t="str">
         <f t="shared" ref="H89:H109" si="3">CONCATENATE("&lt;item key=""",C89,""" anchor=""",B89,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_video_drilldown" anchor="individualtopcontent.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_video_drilldown" anchor="contentinteractions.htm" /&gt;</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -3038,7 +3059,7 @@
         <v>62</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>97</v>
@@ -3049,7 +3070,7 @@
       <c r="F90" s="3"/>
       <c r="H90" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="individualcontentdro.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="contentcontributions.htm" /&gt;</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -3057,7 +3078,7 @@
         <v>72</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>98</v>
@@ -3068,7 +3089,7 @@
       <c r="F91" s="3"/>
       <c r="H91" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="individualcontentint.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="individualtopcontent.htm" /&gt;</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -3076,7 +3097,7 @@
         <v>63</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>99</v>
@@ -3087,20 +3108,20 @@
       <c r="F92" s="3"/>
       <c r="H92" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="individualcontentcon.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="individualcontentdro.htm" /&gt;</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B93" s="5" t="s">
-        <v>282</v>
+      <c r="B93" s="6" t="s">
+        <v>279</v>
       </c>
       <c r="F93" s="3"/>
       <c r="H93" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="" anchor="userandcommunityrepo.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="individualcontentint.htm" /&gt;</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3108,7 +3129,7 @@
         <v>66</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>101</v>
@@ -3119,15 +3140,15 @@
       <c r="F94" s="3"/>
       <c r="H94" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributors.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_contributors" anchor="individualcontentcon.htm" /&gt;</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>67</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>284</v>
+      <c r="B95" s="5" t="s">
+        <v>281</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>102</v>
@@ -3138,7 +3159,7 @@
       <c r="F95" s="3"/>
       <c r="H95" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_overlay" anchor="userandcommunityrepo.htm" /&gt;</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -3146,7 +3167,7 @@
         <v>68</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>103</v>
@@ -3157,14 +3178,16 @@
       <c r="F96" s="3"/>
       <c r="H96" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_syndications" anchor="topcontributors.htm" /&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>69</v>
       </c>
-      <c r="B97" s="6"/>
+      <c r="B97" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="C97" s="6" t="s">
         <v>106</v>
       </c>
@@ -3174,14 +3197,16 @@
       <c r="F97" s="3"/>
       <c r="H97" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="geographicdistributi.htm" /&gt;</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>70</v>
       </c>
-      <c r="B98" s="6"/>
+      <c r="B98" s="6" t="s">
+        <v>284</v>
+      </c>
       <c r="C98" s="6" t="s">
         <v>107</v>
       </c>
@@ -3190,16 +3215,14 @@
       </c>
       <c r="H98" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_map_drilldown" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_drilldown" anchor="topsyndications.htm" /&gt;</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>105</v>
       </c>
-      <c r="B99" s="6" t="s">
-        <v>286</v>
-      </c>
+      <c r="B99" s="6"/>
       <c r="C99" s="6" t="s">
         <v>104</v>
       </c>
@@ -3208,16 +3231,14 @@
       </c>
       <c r="H99" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_user_engagement" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>109</v>
       </c>
-      <c r="B100" s="6" t="s">
-        <v>287</v>
-      </c>
+      <c r="B100" s="6"/>
       <c r="C100" s="6" t="s">
         <v>108</v>
       </c>
@@ -3226,24 +3247,27 @@
       </c>
       <c r="H100" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_user_drilldown" anchor="individualuserengage.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_user_drilldown" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="18.75">
       <c r="A101" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="B101" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="H101" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
+        <v>&lt;item key="" anchor="userengagementreport.htm" /&gt;</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>22</v>
       </c>
-      <c r="B102" s="5" t="s">
-        <v>288</v>
+      <c r="B102" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>137</v>
@@ -3253,16 +3277,13 @@
       </c>
       <c r="H102" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_admin_users" anchor="purchasingalicensefo.htm" /&gt;</v>
+        <v>&lt;item key="section_admin_users" anchor="individualuserengage.htm" /&gt;</v>
       </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>91</v>
       </c>
-      <c r="B103" s="5" t="s">
-        <v>289</v>
-      </c>
       <c r="C103" s="5" t="s">
         <v>90</v>
       </c>
@@ -3271,7 +3292,7 @@
       </c>
       <c r="H103" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
+        <v>&lt;item key="section_user_drilldown" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -3279,7 +3300,7 @@
         <v>56</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>138</v>
@@ -3289,7 +3310,7 @@
       </c>
       <c r="H104" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
+        <v>&lt;item key="section_admin_roles" anchor="purchasingalicensefo.htm" /&gt;</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -3297,7 +3318,7 @@
         <v>23</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>89</v>
@@ -3307,16 +3328,19 @@
       </c>
       <c r="H105" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_role_drilldown" anchor="creatingcustomroles.htm" /&gt;</v>
+        <v>&lt;item key="section_role_drilldown" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="18.75">
       <c r="A106" s="2" t="s">
         <v>145</v>
       </c>
+      <c r="B106" s="5" t="s">
+        <v>289</v>
+      </c>
       <c r="H106" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
+        <v>&lt;item key="" anchor="rolemanagement.htm" /&gt;</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3324,7 +3348,7 @@
         <v>148</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>146</v>
@@ -3334,7 +3358,7 @@
       </c>
       <c r="H107" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_desktop_upload" anchor="theuploadtab.htm" /&gt;</v>
+        <v>&lt;item key="section_desktop_upload" anchor="creatingcustomroles.htm" /&gt;</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="18.75">
@@ -3351,7 +3375,7 @@
         <v>152</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>150</v>
@@ -3366,7 +3390,12 @@
     </row>
     <row r="110" spans="1:8">
       <c r="H110" t="s">
-        <v>293</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="B111" s="5" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
def: 3218 filter and bulk action for category contribution policy
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@83073 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -15,8 +15,138 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+still missing value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+both go to same anchor?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B71" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+there is no peparation between add / edit. Which one should I use?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B95" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+there is no general help for all reports</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B104" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+what is this?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="350">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -1057,13 +1187,22 @@
   </si>
   <si>
     <t>managingschemas.htm</t>
+  </si>
+  <si>
+    <t>change category contribution policy</t>
+  </si>
+  <si>
+    <t>section_cats_cont</t>
+  </si>
+  <si>
+    <t>CategoriesContributionWindow.mxml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1124,6 +1263,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1181,7 +1339,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1208,9 +1366,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1514,11 +1669,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1555,7 +1710,7 @@
       <c r="A3" t="s">
         <v>332</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="5" t="s">
         <v>340</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1573,7 +1728,7 @@
       <c r="A4" t="s">
         <v>336</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="5" t="s">
         <v>341</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1583,7 +1738,7 @@
         <v>334</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H5" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
+        <f t="shared" ref="H4:H67" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
         <v>&lt;item key="section_pne_ipad" anchor="mobilesupport.htm" /&gt;</v>
       </c>
     </row>
@@ -1591,7 +1746,7 @@
       <c r="A5" t="s">
         <v>337</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="5" t="s">
         <v>342</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1619,7 +1774,7 @@
         <v>26</v>
       </c>
       <c r="H6" t="str">
-        <f>CONCATENATE("&lt;item key=""",C6,""" anchor=""",B6,""" /&gt;")</f>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_entries" anchor="entriestab.htm" /&gt;</v>
       </c>
     </row>
@@ -1634,7 +1789,7 @@
         <v>37</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7:H69" si="1">CONCATENATE("&lt;item key=""",C7,""" anchor=""",B7,""" /&gt;")</f>
+        <f t="shared" si="0"/>
         <v>&lt;item key="" anchor="editentrymenus.htm" /&gt;</v>
       </c>
     </row>
@@ -1652,7 +1807,7 @@
         <v>37</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_accesscontrol" anchor="creatinganaccessprof.htm" /&gt;</v>
       </c>
     </row>
@@ -1670,7 +1825,7 @@
         <v>37</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_ads" anchor="addingamidroll.htm" /&gt;</v>
       </c>
     </row>
@@ -1688,7 +1843,7 @@
         <v>37</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_captions" anchor="addingcaptionstoanen.htm" /&gt;</v>
       </c>
     </row>
@@ -1706,7 +1861,7 @@
         <v>37</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_clips" anchor="clippingandtrimmingm.htm" /&gt;</v>
       </c>
     </row>
@@ -1724,7 +1879,7 @@
         <v>37</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_content" anchor="themixestab dz - legacy no? how do I get this tab" /&gt;</v>
       </c>
     </row>
@@ -1742,7 +1897,7 @@
         <v>37</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_metadata" anchor="uploadamediafileands.htm" /&gt;</v>
       </c>
     </row>
@@ -1760,7 +1915,7 @@
         <v>37</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_distribution" anchor="addingadistributorto.htm" /&gt;</v>
       </c>
     </row>
@@ -1778,7 +1933,7 @@
         <v>37</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_flavors" anchor="theflavorstab.htm" /&gt;</v>
       </c>
     </row>
@@ -1796,7 +1951,7 @@
         <v>37</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_replacement" anchor="replacingmedia.htm" /&gt;</v>
       </c>
     </row>
@@ -1814,7 +1969,7 @@
         <v>37</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_live_stream" anchor="configuringthelivest.htm" /&gt;</v>
       </c>
     </row>
@@ -1832,7 +1987,7 @@
         <v>37</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_related" anchor="uploadingandmodifyin.htm" /&gt;</v>
       </c>
     </row>
@@ -1850,7 +2005,7 @@
         <v>37</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_scheduling" anchor="contentscheduling.htm" /&gt;</v>
       </c>
     </row>
@@ -1868,7 +2023,7 @@
         <v>37</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_thumbnails" anchor="troubleshootingtrimm.htm" /&gt;</v>
       </c>
     </row>
@@ -1886,7 +2041,7 @@
         <v>37</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="entry_users" anchor="userstab.htm" /&gt;</v>
       </c>
     </row>
@@ -1905,7 +2060,7 @@
       </c>
       <c r="F22" s="3"/>
       <c r="H22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_download" anchor="downloadfiles.htm" /&gt;</v>
       </c>
     </row>
@@ -1923,7 +2078,7 @@
         <v>115</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_add_entry_tags" anchor="addtags1.htm" /&gt;</v>
       </c>
     </row>
@@ -1941,7 +2096,7 @@
         <v>116</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_remove_entry_tags" anchor="removingtags.htm" /&gt;</v>
       </c>
     </row>
@@ -1959,7 +2114,7 @@
         <v>51</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_bulk_access_control" anchor="setaccesscontrol.htm" /&gt;</v>
       </c>
     </row>
@@ -1977,7 +2132,7 @@
         <v>52</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_bulk_sched" anchor="setscheduling.htm" /&gt;</v>
       </c>
     </row>
@@ -1995,7 +2150,7 @@
         <v>222</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_entry_owner" anchor="changeowner1.htm" /&gt;</v>
       </c>
     </row>
@@ -2013,7 +2168,7 @@
         <v>224</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_entry_remove_cats" anchor="removecategories.htm" /&gt;</v>
       </c>
     </row>
@@ -2031,7 +2186,7 @@
         <v>33</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_add_live_stream" anchor="creatingalivestreami.htm" /&gt;</v>
       </c>
     </row>
@@ -2049,7 +2204,7 @@
         <v>156</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_flavor_dropfolder" anchor="matchfilesfromdropfo.htm" /&gt;</v>
       </c>
     </row>
@@ -2067,7 +2222,7 @@
         <v>164</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_flavor_upload" anchor="uploadfromdesktop.htm" /&gt;</v>
       </c>
     </row>
@@ -2085,7 +2240,7 @@
         <v>164</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_flavor_import" anchor="addvideoaudio.htm" /&gt;</v>
       </c>
     </row>
@@ -2103,7 +2258,7 @@
         <v>164</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_flavor_link" anchor="linktoremotestorage.htm" /&gt;</v>
       </c>
     </row>
@@ -2121,7 +2276,7 @@
         <v>26</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_moderation" anchor="themoderatationtab.htm" /&gt;</v>
       </c>
     </row>
@@ -2139,7 +2294,7 @@
         <v>26</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("&lt;item key=""",C35,""" anchor=""",B35,""" /&gt;")</f>
         <v>&lt;item key="section_playlists" anchor="whatisaplaylist.htm" /&gt;</v>
       </c>
     </row>
@@ -2157,7 +2312,7 @@
         <v>31</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_manual_playlist" anchor="creatingamanualplayl.htm" /&gt;</v>
       </c>
     </row>
@@ -2175,7 +2330,7 @@
         <v>30</v>
       </c>
       <c r="H37" t="str">
-        <f>CONCATENATE("&lt;item key=""",C37,""" anchor=""",B37,""" /&gt;")</f>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_rule_playlist" anchor="creatingarulebasedpl.htm" /&gt;</v>
       </c>
     </row>
@@ -2193,7 +2348,7 @@
         <v>34</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_edit_rule" anchor="definingarule.htm" /&gt;</v>
       </c>
     </row>
@@ -2211,7 +2366,7 @@
         <v>26</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_syndication" anchor="settingupsyndication.htm" /&gt;</v>
       </c>
     </row>
@@ -2229,7 +2384,7 @@
         <v>35</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_ExternalSyndicationPopup" anchor="settingupsyndication.htm" /&gt;</v>
       </c>
     </row>
@@ -2247,7 +2402,7 @@
         <v>36</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_ExternalSyndicationNotification" anchor="kmcpublishertasksfor.htm" /&gt;</v>
       </c>
     </row>
@@ -2265,7 +2420,7 @@
         <v>26</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_categories" anchor="thecategoriestab.htm" /&gt;</v>
       </c>
     </row>
@@ -2283,7 +2438,7 @@
         <v>203</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_category_parent" anchor="addacategory.htm" /&gt;</v>
       </c>
     </row>
@@ -2301,7 +2456,7 @@
         <v>203</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
       </c>
     </row>
@@ -2319,7 +2474,7 @@
         <v>203</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_category_users" anchor="categoryenduserentit.htm" /&gt;</v>
       </c>
     </row>
@@ -2337,7 +2492,7 @@
         <v>203</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_category_subcats" anchor="subcategories.htm" /&gt;</v>
       </c>
     </row>
@@ -2355,7 +2510,7 @@
         <v>208</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_cat_user_permission" anchor="enduseraccesspermiss.htm" /&gt;</v>
       </c>
     </row>
@@ -2373,7 +2528,7 @@
         <v>211</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_cat_user_add" anchor="addacategory.htm" /&gt;</v>
       </c>
     </row>
@@ -2391,7 +2546,7 @@
         <v>213</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
       </c>
     </row>
@@ -2409,7 +2564,7 @@
         <v>115</v>
       </c>
       <c r="H50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
       </c>
     </row>
@@ -2427,7 +2582,7 @@
         <v>116</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
       </c>
     </row>
@@ -2445,7 +2600,7 @@
         <v>227</v>
       </c>
       <c r="H52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
       </c>
     </row>
@@ -2463,7 +2618,7 @@
         <v>230</v>
       </c>
       <c r="H53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_cats_list" anchor="changelisting.htm" /&gt;</v>
       </c>
     </row>
@@ -2481,7 +2636,7 @@
         <v>232</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_cats_access" anchor="changeaccess.htm" /&gt;</v>
       </c>
     </row>
@@ -2499,678 +2654,646 @@
         <v>234</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_cats_owner" anchor="changeowner.htm" /&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="4"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="8"/>
+      <c r="A56" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="C56" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>349</v>
+      </c>
       <c r="H56" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_cats_cont" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H57" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="section_uploads" anchor="youruploads.htm" /&gt;</v>
-      </c>
+      <c r="A57" s="4"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H58" t="str">
-        <f>CONCATENATE("&lt;item key=""",C58,""" anchor=""",B58,""" /&gt;")</f>
-        <v>&lt;item key="section_bulk_log" anchor="bulkuploadlog.htm" /&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_uploads" anchor="youruploads.htm" /&gt;</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_bulk_log" anchor="bulkuploadlog.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_drop_folders" anchor="usingadropfolder.htm" /&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="18.75">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:8" ht="18.75">
+      <c r="A61" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="H60" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H61" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="section_studio_player_list" anchor="playerlist.htm" /&gt;</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_studio_player_list" anchor="playerlist.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
         <v>124</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B63" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D63" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H62" t="str">
-        <f t="shared" si="1"/>
+      <c r="H63" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_studio_player" anchor="editingaplayer.htm" /&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="18.75">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:8" ht="18.75">
+      <c r="A64" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H63" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H64" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="section_acc_overview" anchor="accountsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="section_acc_integration" anchor="integrationsettings.htm" /&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_acc_overview" anchor="accountsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>154</v>
+        <v>17</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>153</v>
+        <v>264</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="section_entitlement_more" anchor="section_entitlement_more" /&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_acc_integration" anchor="integrationsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>240</v>
+        <v>154</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>320</v>
+        <v>153</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>238</v>
+        <v>153</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>239</v>
+        <v>45</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="section_cat_entitlement" anchor="addingentitlementcon.htm" /&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_entitlement_more" anchor="section_entitlement_more" /&gt;</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
+        <v>240</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" ref="H68:H73" si="1">CONCATENATE("&lt;item key=""",C68,""" anchor=""",B68,""" /&gt;")</f>
+        <v>&lt;item key="section_cat_entitlement" anchor="addingentitlementcon.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
         <v>16</v>
       </c>
-      <c r="B68" s="12" t="s">
+      <c r="B69" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D69" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H68" t="str">
+      <c r="H69" t="str">
         <f t="shared" si="1"/>
         <v>&lt;item key="section_acc_access_control" anchor="accesscontrolprofile.htm" /&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
-      <c r="A69" t="s">
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
         <v>18</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B70" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="D70" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H69" t="str">
+      <c r="H70" t="str">
         <f t="shared" si="1"/>
         <v>&lt;item key="section_access_control_profile" anchor="creatinganaccessprof.htm" /&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="B70" s="14" t="s">
+    <row r="71" spans="1:8">
+      <c r="B71" s="5" t="s">
         <v>344</v>
-      </c>
-      <c r="D70" s="8"/>
-      <c r="H70" t="str">
-        <f t="shared" ref="H70:H87" si="2">CONCATENATE("&lt;item key=""",C70,""" anchor=""",B70,""" /&gt;")</f>
-        <v>&lt;item key="" anchor="editinganaccessprof.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="13" t="s">
-        <v>330</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>345</v>
       </c>
       <c r="D71" s="8"/>
       <c r="H71" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="addingorremovingadom.htm" /&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;item key="" anchor="editinganaccessprof.htm" /&gt;</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="D72" s="8"/>
       <c r="H72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
+        <v>&lt;item key="" anchor="addingorremovingadom.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D73" s="8"/>
+      <c r="H73" t="str">
+        <f t="shared" si="1"/>
         <v>&lt;item key="" anchor="addingorremovinggeog.htm" /&gt;</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" t="s">
-        <v>129</v>
-      </c>
-      <c r="B73" s="5" t="s">
+    <row r="74" spans="1:8">
+      <c r="A74" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H73" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_transcoding_def" anchor="addingorremovingipad.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" t="s">
-        <v>130</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="D74" s="8"/>
       <c r="H74" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_transcoding_profiles" anchor="convertingvideosinto.htm" /&gt;</v>
+        <f>CONCATENATE("&lt;item key=""",C74,""" anchor=""",B74,""" /&gt;")</f>
+        <v>&lt;item key="" anchor="addingorremovingipad.htm" /&gt;</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;item key="section_transcoding_profile_edit" anchor="addingatranscodingpr.htm" /&gt;</v>
+        <f t="shared" ref="H75:H93" si="2">CONCATENATE("&lt;item key=""",C75,""" anchor=""",B75,""" /&gt;")</f>
+        <v>&lt;item key="section_acc_transcoding_def" anchor="convertingvideosinto.htm" /&gt;</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>140</v>
+        <v>44</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_transcoding_flavor_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_transcoding_profiles" anchor="addingatranscodingpr.htm" /&gt;</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>48</v>
+        <v>142</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C77" s="6" t="s">
-        <v>132</v>
+      <c r="C77" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_custom_data" anchor="editingandcreatingtr.htm" /&gt;</v>
+        <v>&lt;item key="section_transcoding_profile_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>144</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="C78" s="6"/>
+        <v>141</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="D78" s="8" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="managingschemas.htm" /&gt;</v>
+        <v>&lt;item key="section_transcoding_flavor_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>87</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>269</v>
+        <v>48</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>346</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_custom_data_field" anchor="addingaschema.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_custom_data" anchor="managingschemas.htm" /&gt;</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>133</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="C80" s="6"/>
       <c r="D80" s="8" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_user" anchor="kalturacustommetadat.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="addingaschema.htm" /&gt;</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>134</v>
+        <v>268</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_acc_upgrade" anchor="addingaschema.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="18.75">
-      <c r="A82" s="2" t="s">
-        <v>19</v>
+        <v>&lt;item key="section_custom_data_field" anchor="kalturacustommetadat.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>43</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>270</v>
       </c>
+      <c r="C82" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="H82" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="myusersettings.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_user" anchor="myusersettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="C83" s="6" t="s">
-        <v>100</v>
+      <c r="C83" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_usage" anchor="accountupgrade.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H84" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
+        <v>&lt;item key="section_acc_upgrade" anchor="accountupgrade.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="18.75">
+      <c r="A84" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="4" t="s">
-        <v>57</v>
+      <c r="A85" t="s">
+        <v>20</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>272</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_top_content" anchor="bandwidthusagereport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_usage" anchor="bandwidthusagereport.htm" /&gt;</v>
       </c>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" t="s">
-        <v>58</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H86" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_content_dropoff" anchor="" /&gt;</v>
+      <c r="A86" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" t="s">
-        <v>59</v>
+      <c r="A87" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>273</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_content_interactions" anchor="topcontent.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_content" anchor="topcontent.htm" /&gt;</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>274</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H88" t="str">
-        <f>CONCATENATE("&lt;item key=""",C88,""" anchor=""",B88,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_content_contribution" anchor="contentdropoff.htm" /&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;item key="section_analytics_content_dropoff" anchor="contentdropoff.htm" /&gt;</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>275</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" ref="H89:H109" si="3">CONCATENATE("&lt;item key=""",C89,""" anchor=""",B89,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_video_drilldown" anchor="contentinteractions.htm" /&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;item key="section_analytics_content_interactions" anchor="contentinteractions.htm" /&gt;</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>276</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F90" s="3"/>
       <c r="H90" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="contentcontributions.htm" /&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;item key="section_analytics_content_contribution" anchor="contentcontributions.htm" /&gt;</v>
       </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>277</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F91" s="3"/>
       <c r="H91" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="individualtopcontent.htm" /&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;item key="section_analytics_video_drilldown" anchor="individualtopcontent.htm" /&gt;</v>
       </c>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>278</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>39</v>
       </c>
       <c r="F92" s="3"/>
       <c r="H92" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="individualcontentdro.htm" /&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="individualcontentdro.htm" /&gt;</v>
       </c>
     </row>
     <row r="93" spans="1:8">
-      <c r="A93" s="1" t="s">
-        <v>21</v>
+      <c r="A93" t="s">
+        <v>72</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>279</v>
       </c>
+      <c r="C93" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="F93" s="3"/>
       <c r="H93" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="" anchor="individualcontentint.htm" /&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="individualcontentint.htm" /&gt;</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>280</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="F94" s="3"/>
       <c r="H94" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_top_contributors" anchor="individualcontentcon.htm" /&gt;</v>
+        <f>CONCATENATE("&lt;item key=""",C94,""" anchor=""",B94,""" /&gt;")</f>
+        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="individualcontentcon.htm" /&gt;</v>
       </c>
     </row>
     <row r="95" spans="1:8">
-      <c r="A95" t="s">
-        <v>67</v>
+      <c r="A95" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="C95" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="F95" s="3"/>
       <c r="H95" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_map_overlay" anchor="userandcommunityrepo.htm" /&gt;</v>
+        <f t="shared" ref="H95:H112" si="3">CONCATENATE("&lt;item key=""",C95,""" anchor=""",B95,""" /&gt;")</f>
+        <v>&lt;item key="" anchor="userandcommunityrepo.htm" /&gt;</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>282</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>65</v>
@@ -3178,18 +3301,18 @@
       <c r="F96" s="3"/>
       <c r="H96" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_top_syndications" anchor="topcontributors.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributors.htm" /&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>283</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>65</v>
@@ -3197,210 +3320,234 @@
       <c r="F97" s="3"/>
       <c r="H97" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="geographicdistributi.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>284</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>65</v>
       </c>
+      <c r="F98" s="3"/>
       <c r="H98" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_map_drilldown" anchor="topsyndications.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>105</v>
-      </c>
-      <c r="B99" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="B99" s="14"/>
       <c r="C99" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>65</v>
       </c>
+      <c r="F99" s="3"/>
       <c r="H99" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_user_engagement" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>109</v>
-      </c>
-      <c r="B100" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="B100" s="14"/>
       <c r="C100" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>65</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_user_drilldown" anchor="" /&gt;</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="18.75">
-      <c r="A101" s="2" t="s">
-        <v>71</v>
+        <v>&lt;item key="section_analytics_map_drilldown" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>105</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>285</v>
       </c>
+      <c r="C101" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="H101" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="" anchor="userengagementreport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="C102" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D102" s="10" t="s">
-        <v>55</v>
+      <c r="C102" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_admin_users" anchor="individualuserengage.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
-      <c r="A103" t="s">
-        <v>91</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H103" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_user_drilldown" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_user_drilldown" anchor="individualuserengage.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="18.75">
+      <c r="A103" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:8">
-      <c r="A104" t="s">
-        <v>56</v>
-      </c>
       <c r="B104" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="C104" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="H104" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_admin_roles" anchor="purchasingalicensefo.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="purchasingalicensefo.htm" /&gt;</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>23</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>288</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B105" s="14"/>
       <c r="C105" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D105" s="8" t="s">
-        <v>41</v>
+        <v>137</v>
+      </c>
+      <c r="D105" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="H105" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_role_drilldown" anchor="addingauser.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="18.75">
-      <c r="A106" s="2" t="s">
-        <v>145</v>
+        <v>&lt;item key="section_admin_users" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>91</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="H106" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="" anchor="rolemanagement.htm" /&gt;</v>
+        <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>147</v>
+        <v>138</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_desktop_upload" anchor="creatingcustomroles.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="18.75">
-      <c r="A108" s="2" t="s">
-        <v>149</v>
+        <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>23</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8">
-      <c r="A109" t="s">
+        <v>&lt;item key="section_role_drilldown" anchor="creatingcustomroles.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="18.75">
+      <c r="A109" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" t="s">
+        <v>148</v>
+      </c>
+      <c r="B110" s="14"/>
+      <c r="C110" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H110" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;item key="section_desktop_upload" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="18.75">
+      <c r="A111" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
         <v>152</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B112" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C112" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D109" s="7" t="s">
+      <c r="D112" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="H109" t="str">
+      <c r="H112" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_upload_menu" anchor="theuploadtab.htm" /&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
-      <c r="H110" t="s">
+    <row r="113" spans="8:8">
+      <c r="H113" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
-      <c r="B111" s="5" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fwr: platform reports PRD: implementation, updates to help file, permissions and analytics
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@94109 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -21,7 +21,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="0">
+    <comment ref="B41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B94" authorId="0">
+    <comment ref="B95" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0">
+    <comment ref="B109" authorId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="367">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -958,9 +958,6 @@
     <t>creatingcustomroles.htm</t>
   </si>
   <si>
-    <t>theuploadtab.htm</t>
-  </si>
-  <si>
     <t>&lt;/help&gt;</t>
   </si>
   <si>
@@ -1184,6 +1181,48 @@
   </si>
   <si>
     <t>uploadmedia.htm</t>
+  </si>
+  <si>
+    <t>section_analytics_platform</t>
+  </si>
+  <si>
+    <t>platforms</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>analytics.view.Platform.mxml</t>
+  </si>
+  <si>
+    <t>section_analytics_os</t>
+  </si>
+  <si>
+    <t>operating systems</t>
+  </si>
+  <si>
+    <t>section_analytics_browsers</t>
+  </si>
+  <si>
+    <t>browsers</t>
+  </si>
+  <si>
+    <t>section_analytics_platform_drilldown</t>
+  </si>
+  <si>
+    <t>platform drilldown</t>
+  </si>
+  <si>
+    <t>section_pne_embed</t>
+  </si>
+  <si>
+    <t>embedcodetypes.htm</t>
+  </si>
+  <si>
+    <t>preview and embed - embed types</t>
+  </si>
+  <si>
+    <t>thekalturauploader.htm</t>
   </si>
 </sst>
 </file>
@@ -1672,10 +1711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1702,21 +1741,21 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>306</v>
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("&lt;item key=""",C3,""" anchor=""",B3,""" /&gt;")</f>
@@ -1725,34 +1764,34 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H67" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
+        <f t="shared" ref="H4:H68" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
         <v>&lt;item key="section_pne_ipad" anchor="mobilesupport.htm" /&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -1760,1483 +1799,1478 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
+        <v>365</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B7" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H6" t="str">
+      <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_entries" anchor="entriestable.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="" anchor="editentrymenus.htm" /&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_accesscontrol" anchor="creatinganaccessprof.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="editentrymenus.htm" /&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_ads" anchor="addingamidroll.htm" /&gt;</v>
+        <v>&lt;item key="entry_accesscontrol" anchor="creatinganaccessprof.htm" /&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_captions" anchor="addingcaptionstoanen.htm" /&gt;</v>
+        <v>&lt;item key="entry_ads" anchor="addingamidroll.htm" /&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>295</v>
+        <v>243</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_clips" anchor="clippingandtrimmingm.htm" /&gt;</v>
+        <v>&lt;item key="entry_captions" anchor="addingcaptionstoanen.htm" /&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>314</v>
+        <v>183</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>294</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_content" anchor="themixestab dz - legacy no? how do I get this tab" /&gt;</v>
+        <v>&lt;item key="entry_clips" anchor="clippingandtrimmingm.htm" /&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>185</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>244</v>
+        <v>184</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>313</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_metadata" anchor="uploadamediafileands.htm" /&gt;</v>
+        <v>&lt;item key="entry_content" anchor="themixestab dz - legacy no? how do I get this tab" /&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_distribution" anchor="addingadistributorto.htm" /&gt;</v>
+        <v>&lt;item key="entry_metadata" anchor="uploadamediafileands.htm" /&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_flavors" anchor="theflavorstab.htm" /&gt;</v>
+        <v>&lt;item key="entry_distribution" anchor="addingadistributorto.htm" /&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_replacement" anchor="replacingmedia.htm" /&gt;</v>
+        <v>&lt;item key="entry_flavors" anchor="theflavorstab.htm" /&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_live_stream" anchor="configuringthelivest.htm" /&gt;</v>
+        <v>&lt;item key="entry_replacement" anchor="replacingmedia.htm" /&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>247</v>
+        <v>295</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_related" anchor="uploadingandmodifyin.htm" /&gt;</v>
+        <v>&lt;item key="section_live_stream" anchor="configuringthelivest.htm" /&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_scheduling" anchor="contentscheduling.htm" /&gt;</v>
+        <v>&lt;item key="entry_related" anchor="uploadingandmodifyin.htm" /&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>190</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>320</v>
+        <v>189</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_thumbnails" anchor="choosingathumbnailfo.htm" /&gt;</v>
+        <v>&lt;item key="entry_scheduling" anchor="contentscheduling.htm" /&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>191</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>281</v>
+        <v>190</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>319</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_users" anchor="userstab.htm" /&gt;</v>
+        <v>&lt;item key="entry_thumbnails" anchor="choosingathumbnailfo.htm" /&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>116</v>
+        <v>179</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="3"/>
+        <v>37</v>
+      </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_download" anchor="downloadfiles.htm" /&gt;</v>
+        <v>&lt;item key="entry_users" anchor="userstab.htm" /&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>193</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>321</v>
+        <v>192</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>281</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>114</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F23" s="3"/>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_entry_tags" anchor="editaddtagstoandentr.htm" /&gt;</v>
+        <v>&lt;item key="section_download" anchor="downloadfiles.htm" /&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_remove_entry_tags" anchor="editremovetagsfroman.htm" /&gt;</v>
+        <v>&lt;item key="section_add_entry_tags" anchor="editaddtagstoandentr.htm" /&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>283</v>
+        <v>194</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>321</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_access_control" anchor="setaccesscontrol.htm" /&gt;</v>
+        <v>&lt;item key="section_remove_entry_tags" anchor="editremovetagsfroman.htm" /&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_sched" anchor="setscheduling.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_access_control" anchor="setaccesscontrol.htm" /&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>220</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>323</v>
+        <v>196</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>283</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>219</v>
+        <v>120</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>221</v>
+        <v>52</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entry_owner" anchor="changeentryowner.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_sched" anchor="setscheduling.htm" /&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entry_remove_cats" anchor="editremovecategories.htm" /&gt;</v>
+        <v>&lt;item key="section_entry_owner" anchor="changeentryowner.htm" /&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>285</v>
+        <v>224</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>323</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>112</v>
+        <v>222</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>33</v>
+        <v>223</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_live_stream" anchor="creatingalivestreami.htm" /&gt;</v>
+        <v>&lt;item key="section_entry_remove_cats" anchor="editremovecategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_add_live_stream" anchor="creatingalivestreami.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
         <v>156</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="B31" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D31" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="H30" t="str">
+      <c r="H31" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_flavor_dropfolder" anchor="matchfilesfromdropfo.htm" /&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="15" t="s">
+    <row r="32" spans="1:8">
+      <c r="A32" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_upload" anchor="uploadfromdesktop.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>162</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>163</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_import" anchor="importfiles.htm" /&gt;</v>
+        <v>&lt;item key="section_flavor_upload" anchor="uploadfromdesktop.htm" /&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>161</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>297</v>
+        <v>162</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>324</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>163</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
+        <v>&lt;item key="section_flavor_import" anchor="importfiles.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_flavor_link" anchor="linktoremotestorage.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>326</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_moderation" anchor="themoderationtab.htm" /&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H35" t="str">
-        <f>CONCATENATE("&lt;item key=""",C35,""" anchor=""",B35,""" /&gt;")</f>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_moderation" anchor="themoderationtab.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" t="str">
+        <f>CONCATENATE("&lt;item key=""",C36,""" anchor=""",B36,""" /&gt;")</f>
         <v>&lt;item key="section_playlists" anchor="playliststab.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H36" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_manual_playlist" anchor="creatingamanualplayl.htm" /&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_rule_playlist" anchor="creatingarulebasedpl.htm" /&gt;</v>
+        <v>&lt;item key="section_manual_playlist" anchor="creatingamanualplayl.htm" /&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_rule_playlist" anchor="creatingarulebasedpl.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H38" t="str">
+      <c r="H39" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_edit_rule" anchor="definingarule.htm" /&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H39" t="str">
+      <c r="H40" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_syndication" anchor="settingupsyndication.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" t="s">
-        <v>253</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H40" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_ExternalSyndicationPopup" anchor="googlewebmastertasks.htm" /&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
+        <v>253</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_ExternalSyndicationPopup" anchor="googlewebmastertasks.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B42" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D42" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H41" t="str">
+      <c r="H42" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_ExternalSyndicationNotification" anchor="kmcpublishertasksfor.htm" /&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="C42" s="5" t="s">
+      <c r="B43" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H42" t="str">
+      <c r="H43" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_categories" anchor="categoriestable.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>330</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="H43" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_parent" anchor="addingeditingaspecif.htm" /&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>256</v>
+        <v>198</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>329</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>202</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
+        <v>&lt;item key="section_category_parent" anchor="addingeditingaspecif.htm" /&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>331</v>
+        <v>199</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>256</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>202</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_users" anchor="editingtheentitlemen.htm" /&gt;</v>
+        <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>332</v>
+        <v>200</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>330</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>202</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_subcats" anchor="reorderingsubcategor.htm" /&gt;</v>
+        <v>&lt;item key="section_category_users" anchor="editingtheentitlemen.htm" /&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_permission" anchor="categorysentitlement.htm" /&gt;</v>
+        <v>&lt;item key="section_category_subcats" anchor="reorderingsubcategor.htm" /&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>330</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>209</v>
+        <v>332</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_add" anchor="addingeditingaspecif.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_user_permission" anchor="categorysentitlement.htm" /&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>287</v>
+        <v>211</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>329</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_user_add" anchor="addingeditingaspecif.htm" /&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
+        <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="4" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>226</v>
+        <v>115</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
+        <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>337</v>
+        <v>227</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_list" anchor="changecategorylistin.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>336</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_access" anchor="changecontentprivacy.htm" /&gt;</v>
+        <v>&lt;item key="section_cats_list" anchor="changecategorylistin.htm" /&gt;</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_owner" anchor="changecategoryowner.htm" /&gt;</v>
+        <v>&lt;item key="section_cats_access" anchor="changecontentprivacy.htm" /&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_cats_owner" anchor="changecategoryowner.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B56" s="16" t="s">
-        <v>335</v>
-      </c>
-      <c r="C56" s="6" t="s">
+      <c r="D57" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="D56" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="H56" t="str">
+      <c r="H57" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_cats_cont" anchor="changecontributionpo.htm" /&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="4"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="8"/>
-    </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H58" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_uploads" anchor="youruploads.htm" /&gt;</v>
-      </c>
+      <c r="A58" s="4"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_log" anchor="bulkuploadlog.htm" /&gt;</v>
+        <v>&lt;item key="section_uploads" anchor="youruploads.htm" /&gt;</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
+        <v>&lt;item key="section_bulk_log" anchor="bulkuploadlog.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;item key="section_drop_folders" anchor="usingadropfolder.htm" /&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="18.75">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:8" ht="18.75">
+      <c r="A62" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H62" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_studio_player_list" anchor="playerlist.htm" /&gt;</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_studio_player_list" anchor="playerlist.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B64" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C64" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D64" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H63" t="str">
+      <c r="H64" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_studio_player" anchor="editingaplayer.htm" /&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="18.75">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:8" ht="18.75">
+      <c r="A65" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" t="s">
-        <v>15</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H65" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_acc_overview" anchor="accountsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_acc_integration" anchor="integrationsettings.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_overview" anchor="accountsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>153</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>338</v>
+        <v>17</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>260</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entitlement_more" anchor="entitlementsettings.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_integration" anchor="integrationsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>239</v>
+        <v>153</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>238</v>
+        <v>45</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" ref="H68:H72" si="1">CONCATENATE("&lt;item key=""",C68,""" anchor=""",B68,""" /&gt;")</f>
-        <v>&lt;item key="section_cat_entitlement" anchor="editingtheentitlemen.htm" /&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_entitlement_more" anchor="entitlementsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
+        <v>239</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" ref="H69:H73" si="1">CONCATENATE("&lt;item key=""",C69,""" anchor=""",B69,""" /&gt;")</f>
+        <v>&lt;item key="section_cat_entitlement" anchor="editingtheentitlemen.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
         <v>16</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="C69" s="5" t="s">
+      <c r="B70" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D69" s="9" t="s">
+      <c r="D70" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H69" t="str">
+      <c r="H70" t="str">
         <f t="shared" si="1"/>
         <v>&lt;item key="section_acc_access_control" anchor="accesscontrolprofile.htm" /&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
-      <c r="A70" t="s">
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
         <v>18</v>
       </c>
-      <c r="B70" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="C70" s="5" t="s">
+      <c r="B71" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D71" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H70" t="str">
+      <c r="H71" t="str">
         <f t="shared" si="1"/>
         <v>&lt;item key="section_access_control_profile" anchor="editinganaccessprofi.htm" /&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="D71" s="8"/>
-      <c r="H71" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="addingorremovingadom.htm" /&gt;</v>
-      </c>
-    </row>
     <row r="72" spans="1:8">
       <c r="A72" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
       <c r="D72" s="8"/>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="addingorremovinggeog.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="addingorremovingadom.htm" /&gt;</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D73" s="8"/>
       <c r="H73" t="str">
-        <f>CONCATENATE("&lt;item key=""",C73,""" anchor=""",B73,""" /&gt;")</f>
+        <f t="shared" si="1"/>
+        <v>&lt;item key="" anchor="addingorremovinggeog.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D74" s="8"/>
+      <c r="H74" t="str">
+        <f>CONCATENATE("&lt;item key=""",C74,""" anchor=""",B74,""" /&gt;")</f>
         <v>&lt;item key="" anchor="addingorremovingipad.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" t="s">
-        <v>128</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H74" t="str">
-        <f t="shared" ref="H74:H92" si="2">CONCATENATE("&lt;item key=""",C74,""" anchor=""",B74,""" /&gt;")</f>
-        <v>&lt;item key="section_acc_transcoding_def" anchor="convertingvideosinto.htm" /&gt;</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>44</v>
       </c>
       <c r="H75" t="str">
+        <f t="shared" ref="H75:H93" si="2">CONCATENATE("&lt;item key=""",C75,""" anchor=""",B75,""" /&gt;")</f>
+        <v>&lt;item key="section_acc_transcoding_def" anchor="convertingvideosinto.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H76" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_acc_transcoding_profiles" anchor="addingatranscodingpr.htm" /&gt;</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
-      <c r="A76" t="s">
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
         <v>141</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B77" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D77" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H76" t="str">
+      <c r="H77" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_transcoding_profile_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
-      <c r="A77" t="s">
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
         <v>140</v>
       </c>
-      <c r="B77" s="14" t="s">
-        <v>340</v>
-      </c>
-      <c r="C77" s="5" t="s">
+      <c r="B78" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="C78" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D78" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="H77" t="str">
+      <c r="H78" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_transcoding_flavor_edit" anchor="editingoptionsforfla.htm" /&gt;</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
-      <c r="A78" t="s">
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
         <v>48</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B79" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D79" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H78" t="str">
+      <c r="H79" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_acc_custom_data" anchor="addingaschema.htm" /&gt;</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
-      <c r="A79" t="s">
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
         <v>143</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B80" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="8" t="s">
+      <c r="C80" s="6"/>
+      <c r="D80" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H79" t="str">
+      <c r="H80" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="" anchor="kalturacustommetadat.htm" /&gt;</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
-      <c r="A80" t="s">
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="16" t="s">
-        <v>341</v>
-      </c>
-      <c r="C80" s="6" t="s">
+      <c r="B81" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D81" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H80" t="str">
+      <c r="H81" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_custom_data_field" anchor="addingcustomdatafiel.htm" /&gt;</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
-      <c r="A81" t="s">
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
         <v>43</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B82" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D82" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H81" t="str">
+      <c r="H82" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_acc_user" anchor="myusersettings.htm" /&gt;</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" t="s">
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
         <v>134</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B83" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C83" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D83" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="H82" t="str">
+      <c r="H83" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_acc_upgrade" anchor="accountupgrade.htm" /&gt;</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="18.75">
-      <c r="A83" s="2" t="s">
+    <row r="84" spans="1:8" ht="18.75">
+      <c r="A84" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
-      <c r="A84" t="s">
+    <row r="85" spans="1:8">
+      <c r="A85" t="s">
         <v>20</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B85" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="D85" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H84" t="str">
+      <c r="H85" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_usage" anchor="bandwidthusagereport.htm" /&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:8">
+      <c r="A86" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B86" s="14" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="4" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="B86" s="6" t="s">
+      <c r="B87" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="D87" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H86" t="str">
+      <c r="H87" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_top_content" anchor="topcontent.htm" /&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
-      <c r="A87" t="s">
+    <row r="88" spans="1:8">
+      <c r="A88" t="s">
         <v>57</v>
       </c>
-      <c r="B87" s="16" t="s">
-        <v>344</v>
-      </c>
-      <c r="C87" s="6" t="s">
+      <c r="B88" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D87" s="8" t="s">
+      <c r="D88" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H87" t="str">
+      <c r="H88" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_content_dropoff" anchor="contentdropoffreport.htm" /&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
-      <c r="A88" t="s">
+    <row r="89" spans="1:8">
+      <c r="A89" t="s">
         <v>58</v>
       </c>
-      <c r="B88" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="C88" s="6" t="s">
+      <c r="B89" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D88" s="8" t="s">
+      <c r="D89" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H88" t="str">
+      <c r="H89" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_content_interactions" anchor="contentinteractionsr.htm" /&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
-      <c r="A89" t="s">
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
         <v>59</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B90" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C90" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D89" s="8" t="s">
+      <c r="D90" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H89" t="str">
+      <c r="H90" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_content_contribution" anchor="contentcontributions.htm" /&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
-      <c r="A90" t="s">
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
         <v>60</v>
       </c>
-      <c r="B90" s="16" t="s">
-        <v>346</v>
-      </c>
-      <c r="C90" s="6" t="s">
+      <c r="B91" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D90" s="8" t="s">
+      <c r="D91" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H90" t="str">
+      <c r="H91" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_video_drilldown" anchor="specificentrymediaso.htm" /&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="A91" t="s">
-        <v>61</v>
-      </c>
-      <c r="B91" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F91" s="3"/>
-      <c r="H91" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="specificentrycontent.htm" /&gt;</v>
-      </c>
-    </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>39</v>
@@ -3244,69 +3278,69 @@
       <c r="F92" s="3"/>
       <c r="H92" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="specificcontentinter.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="specificentrycontent.htm" /&gt;</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>39</v>
       </c>
       <c r="F93" s="3"/>
       <c r="H93" t="str">
-        <f>CONCATENATE("&lt;item key=""",C93,""" anchor=""",B93,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="specificentrymediaso.htm" /&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="specificcontentinter.htm" /&gt;</v>
       </c>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>271</v>
+      <c r="A94" t="s">
+        <v>62</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="F94" s="3"/>
       <c r="H94" t="str">
-        <f t="shared" ref="H94:H111" si="3">CONCATENATE("&lt;item key=""",C94,""" anchor=""",B94,""" /&gt;")</f>
-        <v>&lt;item key="" anchor="userandcommunityrepo.htm" /&gt;</v>
+        <f>CONCATENATE("&lt;item key=""",C94,""" anchor=""",B94,""" /&gt;")</f>
+        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="specificentrymediaso.htm" /&gt;</v>
       </c>
     </row>
     <row r="95" spans="1:8">
-      <c r="A95" t="s">
-        <v>65</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>349</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>64</v>
+      <c r="A95" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>271</v>
       </c>
       <c r="F95" s="3"/>
       <c r="H95" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributorsrepor.htm" /&gt;</v>
+        <f t="shared" ref="H95:H117" si="3">CONCATENATE("&lt;item key=""",C95,""" anchor=""",B95,""" /&gt;")</f>
+        <v>&lt;item key="" anchor="userandcommunityrepo.htm" /&gt;</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>66</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>272</v>
+        <v>65</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>348</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>64</v>
@@ -3314,18 +3348,18 @@
       <c r="F96" s="3"/>
       <c r="H96" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributorsrepor.htm" /&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>64</v>
@@ -3333,18 +3367,18 @@
       <c r="F97" s="3"/>
       <c r="H97" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>68</v>
-      </c>
-      <c r="B98" s="14" t="s">
-        <v>350</v>
+        <v>67</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>273</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>64</v>
@@ -3352,195 +3386,286 @@
       <c r="F98" s="3"/>
       <c r="H98" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="specificsyndicatorre.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>64</v>
       </c>
+      <c r="F99" s="3"/>
       <c r="H99" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_map_drilldown" anchor="specificgeographicre.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="specificsyndicatorre.htm" /&gt;</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>104</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>274</v>
+        <v>69</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>350</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>64</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_drilldown" anchor="specificgeographicre.htm" /&gt;</v>
       </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>352</v>
+        <v>274</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>64</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="3"/>
+        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H102" t="str">
+        <f t="shared" si="3"/>
         <v>&lt;item key="section_analytics_user_drilldown" anchor="specificuserengageme.htm" /&gt;</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="18.75">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:8">
+      <c r="A103" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="8"/>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>354</v>
+      </c>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="H104" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;item key="section_analytics_platform" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>358</v>
+      </c>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="H105" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;item key="section_analytics_os" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>360</v>
+      </c>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="H106" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;item key="section_analytics_browsers" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>362</v>
+      </c>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="H107" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;item key="section_analytics_platform_drilldown" anchor="" /&gt;</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="18.75">
+      <c r="A108" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
-      <c r="H103" t="str">
+    <row r="109" spans="1:8">
+      <c r="H109" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="" anchor="" /&gt;</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
-      <c r="A104" t="s">
+    <row r="110" spans="1:8">
+      <c r="A110" t="s">
         <v>22</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B110" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C104" s="5" t="s">
+      <c r="C110" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D104" s="10" t="s">
+      <c r="D110" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H104" t="str">
+      <c r="H110" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_admin_users" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
-      <c r="A105" t="s">
+    <row r="111" spans="1:8">
+      <c r="A111" t="s">
         <v>90</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B111" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C105" s="5" t="s">
+      <c r="C111" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="D111" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H105" t="str">
+      <c r="H111" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
-      <c r="A106" t="s">
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
         <v>56</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B112" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="C106" s="5" t="s">
+      <c r="C112" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D106" s="10" t="s">
+      <c r="D112" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H106" t="str">
+      <c r="H112" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
-      <c r="A107" t="s">
+    <row r="113" spans="1:8">
+      <c r="A113" t="s">
         <v>23</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B113" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="C113" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D107" s="8" t="s">
+      <c r="D113" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H107" t="str">
+      <c r="H113" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_role_drilldown" anchor="creatingcustomroles.htm" /&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="18.75">
-      <c r="A108" s="2" t="s">
+    <row r="114" spans="1:8" ht="18.75">
+      <c r="A114" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
-      <c r="A109" t="s">
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
         <v>147</v>
       </c>
-      <c r="B109" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="C109" s="5" t="s">
+      <c r="B115" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C115" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D109" s="7" t="s">
+      <c r="D115" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="H109" t="str">
+      <c r="H115" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_desktop_upload" anchor="uploadmedia.htm" /&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="18.75">
-      <c r="A110" s="2" t="s">
+    <row r="116" spans="1:8" ht="18.75">
+      <c r="A116" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
-      <c r="A111" t="s">
+    <row r="117" spans="1:8">
+      <c r="A117" t="s">
         <v>151</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B117" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H117" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;item key="section_upload_menu" anchor="thekalturauploader.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="H118" t="s">
         <v>278</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="H111" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_upload_menu" anchor="theuploadtab.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
-      <c r="H112" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fwr: add different help anchors for different live stream types
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@96440 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B41" authorId="0">
+    <comment ref="B43" authorId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B95" authorId="0">
+    <comment ref="B97" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B109" authorId="0">
+    <comment ref="B111" authorId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="371">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -148,9 +148,6 @@
     <t>edit entry (Drill down)</t>
   </si>
   <si>
-    <t>new live stream</t>
-  </si>
-  <si>
     <t xml:space="preserve">manual playlist </t>
   </si>
   <si>
@@ -1223,13 +1220,28 @@
   </si>
   <si>
     <t>thekalturauploader.htm</t>
+  </si>
+  <si>
+    <t>new live stream (rtmp)</t>
+  </si>
+  <si>
+    <t>new live stream (Akamai hds / hls)</t>
+  </si>
+  <si>
+    <t>new live stream (manual)</t>
+  </si>
+  <si>
+    <t>section_add_live_stream_ak</t>
+  </si>
+  <si>
+    <t>section_add_live_stream_man</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1309,13 +1321,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1373,7 +1378,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1396,10 +1401,8 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1711,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1730,10 +1733,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75">
@@ -1741,21 +1744,21 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>304</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>305</v>
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("&lt;item key=""",C3,""" anchor=""",B3,""" /&gt;")</f>
@@ -1764,34 +1767,34 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H68" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
+        <f t="shared" ref="H4:H70" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
         <v>&lt;item key="section_pne_ipad" anchor="mobilesupport.htm" /&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -1800,16 +1803,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1817,13 +1820,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -1835,10 +1838,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -1847,16 +1850,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -1865,16 +1868,16 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -1883,16 +1886,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -1901,16 +1904,16 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -1919,16 +1922,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -1937,16 +1940,16 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -1955,16 +1958,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -1973,16 +1976,16 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -1991,16 +1994,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -2009,16 +2012,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -2027,16 +2030,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -2045,16 +2048,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -2063,16 +2066,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>190</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>319</v>
+        <v>189</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>318</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -2081,16 +2084,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -2099,16 +2102,16 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="3"/>
       <c r="H23" t="str">
@@ -2118,16 +2121,16 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>193</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>320</v>
+        <v>192</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>319</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -2136,16 +2139,16 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>321</v>
+        <v>193</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>320</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -2154,16 +2157,16 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -2172,16 +2175,16 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -2190,16 +2193,16 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>322</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -2208,16 +2211,16 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>224</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>323</v>
+        <v>223</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>322</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -2226,16 +2229,16 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>366</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -2244,1428 +2247,1460 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>156</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>285</v>
-      </c>
+        <v>367</v>
+      </c>
+      <c r="B31" s="6"/>
       <c r="C31" s="5" t="s">
-        <v>154</v>
+        <v>369</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>155</v>
+        <v>32</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_dropfolder" anchor="matchfilesfromdropfo.htm" /&gt;</v>
+        <v>&lt;item key="section_add_live_stream_ak" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>249</v>
-      </c>
+      <c r="A32" t="s">
+        <v>368</v>
+      </c>
+      <c r="B32" s="6"/>
       <c r="C32" s="5" t="s">
-        <v>157</v>
+        <v>370</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>163</v>
+        <v>32</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_upload" anchor="uploadfromdesktop.htm" /&gt;</v>
+        <v>&lt;item key="section_add_live_stream_man" anchor="" /&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_flavor_dropfolder" anchor="matchfilesfromdropfo.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_flavor_upload" anchor="uploadfromdesktop.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_flavor_import" anchor="importfiles.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_flavor_link" anchor="linktoremotestorage.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="H33" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_import" anchor="importfiles.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>161</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="H34" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_link" anchor="linktoremotestorage.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="14" t="s">
+      <c r="C37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_moderation" anchor="themoderationtab.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_moderation" anchor="themoderationtab.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>326</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H36" t="str">
-        <f>CONCATENATE("&lt;item key=""",C36,""" anchor=""",B36,""" /&gt;")</f>
+      <c r="D38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" t="str">
+        <f>CONCATENATE("&lt;item key=""",C38,""" anchor=""",B38,""" /&gt;")</f>
         <v>&lt;item key="section_playlists" anchor="playliststab.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H37" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_manual_playlist" anchor="creatingamanualplayl.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_rule_playlist" anchor="creatingarulebasedpl.htm" /&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>252</v>
+        <v>8</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>249</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_edit_rule" anchor="definingarule.htm" /&gt;</v>
+        <v>&lt;item key="section_manual_playlist" anchor="creatingamanualplayl.htm" /&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="1" t="s">
-        <v>5</v>
+      <c r="A40" t="s">
+        <v>9</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_syndication" anchor="settingupsyndication.htm" /&gt;</v>
+        <v>&lt;item key="section_rule_playlist" anchor="creatingarulebasedpl.htm" /&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>253</v>
+        <v>23</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>327</v>
+        <v>251</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>110</v>
       </c>
       <c r="D41" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_edit_rule" anchor="definingarule.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_syndication" anchor="settingupsyndication.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>252</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_ExternalSyndicationPopup" anchor="googlewebmastertasks.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H41" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_ExternalSyndicationPopup" anchor="googlewebmastertasks.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H42" t="str">
+      <c r="H44" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_ExternalSyndicationNotification" anchor="kmcpublishertasksfor.htm" /&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="C43" s="5" t="s">
+    <row r="45" spans="1:8">
+      <c r="A45" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H43" t="str">
+      <c r="B45" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H45" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_categories" anchor="categoriestable.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>329</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="H44" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_parent" anchor="addingeditingaspecif.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="H45" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>330</v>
+        <v>197</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>328</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_users" anchor="editingtheentitlemen.htm" /&gt;</v>
+        <v>&lt;item key="section_category_parent" anchor="addingeditingaspecif.htm" /&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B47" s="16" t="s">
-        <v>331</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>202</v>
-      </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_subcats" anchor="reorderingsubcategor.htm" /&gt;</v>
+        <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>332</v>
+        <v>199</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>329</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_permission" anchor="categorysentitlement.htm" /&gt;</v>
+        <v>&lt;item key="section_category_users" anchor="editingtheentitlemen.htm" /&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>329</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>209</v>
+        <v>200</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>204</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_add" anchor="addingeditingaspecif.htm" /&gt;</v>
+        <v>&lt;item key="section_category_subcats" anchor="reorderingsubcategor.htm" /&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>213</v>
+        <v>331</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_user_permission" anchor="categorysentitlement.htm" /&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>287</v>
+        <v>328</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>114</v>
+        <v>209</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_user_add" anchor="addingeditingaspecif.htm" /&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>115</v>
+        <v>211</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="4" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>226</v>
+        <v>113</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
+        <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>336</v>
+        <v>217</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_list" anchor="changecategorylistin.htm" /&gt;</v>
+        <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>335</v>
+        <v>226</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>288</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_access" anchor="changecontentprivacy.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>333</v>
+        <v>233</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>335</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_owner" anchor="changecategoryowner.htm" /&gt;</v>
+        <v>&lt;item key="section_cats_list" anchor="changecategorylistin.htm" /&gt;</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_cats_access" anchor="changecontentprivacy.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_cats_owner" anchor="changecategoryowner.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B57" s="16" t="s">
-        <v>334</v>
-      </c>
-      <c r="C57" s="6" t="s">
+      <c r="D59" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="D57" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="H57" t="str">
+      <c r="H59" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_cats_cont" anchor="changecontributionpo.htm" /&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="4"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="8"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H59" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_uploads" anchor="youruploads.htm" /&gt;</v>
-      </c>
-    </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H60" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_log" anchor="bulkuploadlog.htm" /&gt;</v>
-      </c>
+      <c r="A60" s="4"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C61" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_uploads" anchor="youruploads.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_bulk_log" anchor="bulkuploadlog.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H61" t="str">
+      <c r="B63" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H63" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_drop_folders" anchor="usingadropfolder.htm" /&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="18.75">
-      <c r="A62" s="2" t="s">
+    <row r="64" spans="1:8" ht="18.75">
+      <c r="A64" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" t="s">
-        <v>13</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H63" t="str">
+      <c r="B65" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" t="str">
         <f t="shared" si="0"/>
         <v>&lt;item key="section_studio_player_list" anchor="playerlist.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" t="s">
-        <v>123</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H64" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_studio_player" anchor="editingaplayer.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="18.75">
-      <c r="A65" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_acc_overview" anchor="accountsettings.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" t="s">
-        <v>17</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H67" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_acc_integration" anchor="integrationsettings.htm" /&gt;</v>
+        <v>&lt;item key="section_studio_player" anchor="editingaplayer.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="18.75">
+      <c r="A67" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>153</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>337</v>
+        <v>14</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>258</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entitlement_more" anchor="entitlementsettings.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_overview" anchor="accountsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>239</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>330</v>
+        <v>16</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>237</v>
+        <v>124</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>238</v>
+        <v>44</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" ref="H69:H73" si="1">CONCATENATE("&lt;item key=""",C69,""" anchor=""",B69,""" /&gt;")</f>
-        <v>&lt;item key="section_cat_entitlement" anchor="editingtheentitlemen.htm" /&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_acc_integration" anchor="integrationsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>16</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>297</v>
+        <v>152</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>336</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>47</v>
+        <v>151</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="H70" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_entitlement_more" anchor="entitlementsettings.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>238</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" ref="H71:H75" si="1">CONCATENATE("&lt;item key=""",C71,""" anchor=""",B71,""" /&gt;")</f>
+        <v>&lt;item key="section_cat_entitlement" anchor="editingtheentitlemen.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H72" t="str">
         <f t="shared" si="1"/>
         <v>&lt;item key="section_acc_access_control" anchor="accesscontrolprofile.htm" /&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
-      <c r="A71" t="s">
-        <v>18</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H71" t="str">
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>17</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H73" t="str">
         <f t="shared" si="1"/>
         <v>&lt;item key="section_access_control_profile" anchor="editinganaccessprofi.htm" /&gt;</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="D72" s="8"/>
-      <c r="H72" t="str">
+    <row r="74" spans="1:8">
+      <c r="A74" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D74" s="8"/>
+      <c r="H74" t="str">
         <f t="shared" si="1"/>
         <v>&lt;item key="" anchor="addingorremovingadom.htm" /&gt;</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="D73" s="8"/>
-      <c r="H73" t="str">
+    <row r="75" spans="1:8">
+      <c r="A75" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D75" s="8"/>
+      <c r="H75" t="str">
         <f t="shared" si="1"/>
         <v>&lt;item key="" anchor="addingorremovinggeog.htm" /&gt;</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="D74" s="8"/>
-      <c r="H74" t="str">
-        <f>CONCATENATE("&lt;item key=""",C74,""" anchor=""",B74,""" /&gt;")</f>
+    <row r="76" spans="1:8">
+      <c r="A76" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="D76" s="8"/>
+      <c r="H76" t="str">
+        <f>CONCATENATE("&lt;item key=""",C76,""" anchor=""",B76,""" /&gt;")</f>
         <v>&lt;item key="" anchor="addingorremovingipad.htm" /&gt;</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
-      <c r="A75" t="s">
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>127</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H77" t="str">
+        <f t="shared" ref="H77:H95" si="2">CONCATENATE("&lt;item key=""",C77,""" anchor=""",B77,""" /&gt;")</f>
+        <v>&lt;item key="section_acc_transcoding_def" anchor="convertingvideosinto.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
         <v>128</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="C75" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H75" t="str">
-        <f t="shared" ref="H75:H93" si="2">CONCATENATE("&lt;item key=""",C75,""" anchor=""",B75,""" /&gt;")</f>
-        <v>&lt;item key="section_acc_transcoding_def" anchor="convertingvideosinto.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="A76" t="s">
+      <c r="C78" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H76" t="str">
+      <c r="D78" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H78" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_acc_transcoding_profiles" anchor="addingatranscodingpr.htm" /&gt;</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
-      <c r="A77" t="s">
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>140</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C79" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H77" t="str">
+      <c r="D79" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H79" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_transcoding_profile_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
-      <c r="A78" t="s">
-        <v>140</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="C78" s="5" t="s">
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D78" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="H78" t="str">
+      <c r="H80" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_transcoding_flavor_edit" anchor="editingoptionsforfla.htm" /&gt;</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
-      <c r="A79" t="s">
-        <v>48</v>
-      </c>
-      <c r="B79" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H79" t="str">
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>47</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H81" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_acc_custom_data" anchor="addingaschema.htm" /&gt;</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
-      <c r="A80" t="s">
-        <v>143</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H80" t="str">
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H82" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="" anchor="kalturacustommetadat.htm" /&gt;</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
-      <c r="A81" t="s">
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B81" s="16" t="s">
-        <v>340</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H81" t="str">
+      <c r="H83" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_custom_data_field" anchor="addingcustomdatafiel.htm" /&gt;</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" t="s">
-        <v>43</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D82" s="8" t="s">
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
         <v>42</v>
       </c>
-      <c r="H82" t="str">
+      <c r="B84" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H84" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_acc_user" anchor="myusersettings.htm" /&gt;</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
-      <c r="A83" t="s">
+    <row r="85" spans="1:8">
+      <c r="A85" t="s">
+        <v>133</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D85" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H83" t="str">
+      <c r="H85" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_acc_upgrade" anchor="accountupgrade.htm" /&gt;</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="18.75">
-      <c r="A84" s="2" t="s">
+    <row r="86" spans="1:8" ht="18.75">
+      <c r="A86" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85" t="s">
-        <v>20</v>
-      </c>
-      <c r="B85" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H85" t="str">
+      <c r="B87" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H87" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_usage" anchor="bandwidthusagereport.htm" /&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B86" s="14" t="s">
+    <row r="88" spans="1:8">
+      <c r="A88" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="4" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H87" t="str">
+      <c r="B89" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H89" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_top_content" anchor="topcontent.htm" /&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
-      <c r="A88" t="s">
-        <v>57</v>
-      </c>
-      <c r="B88" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D88" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H88" t="str">
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>56</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H90" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_content_dropoff" anchor="contentdropoffreport.htm" /&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
-      <c r="A89" t="s">
-        <v>58</v>
-      </c>
-      <c r="B89" s="16" t="s">
-        <v>344</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H89" t="str">
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>57</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H91" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_content_interactions" anchor="contentinteractionsr.htm" /&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
-      <c r="A90" t="s">
-        <v>59</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H90" t="str">
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>58</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H92" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_content_contribution" anchor="contentcontributions.htm" /&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="A91" t="s">
-        <v>60</v>
-      </c>
-      <c r="B91" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H91" t="str">
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>59</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H93" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_video_drilldown" anchor="specificentrymediaso.htm" /&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
-      <c r="A92" t="s">
-        <v>61</v>
-      </c>
-      <c r="B92" s="16" t="s">
-        <v>346</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F92" s="3"/>
-      <c r="H92" t="str">
+    <row r="94" spans="1:8">
+      <c r="A94" t="s">
+        <v>60</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F94" s="3"/>
+      <c r="H94" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="specificentrycontent.htm" /&gt;</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
-      <c r="A93" t="s">
-        <v>71</v>
-      </c>
-      <c r="B93" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F93" s="3"/>
-      <c r="H93" t="str">
+    <row r="95" spans="1:8">
+      <c r="A95" t="s">
+        <v>70</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F95" s="3"/>
+      <c r="H95" t="str">
         <f t="shared" si="2"/>
         <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="specificcontentinter.htm" /&gt;</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
-      <c r="A94" t="s">
-        <v>62</v>
-      </c>
-      <c r="B94" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F94" s="3"/>
-      <c r="H94" t="str">
-        <f>CONCATENATE("&lt;item key=""",C94,""" anchor=""",B94,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="specificentrymediaso.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="F95" s="3"/>
-      <c r="H95" t="str">
-        <f t="shared" ref="H95:H117" si="3">CONCATENATE("&lt;item key=""",C95,""" anchor=""",B95,""" /&gt;")</f>
-        <v>&lt;item key="" anchor="userandcommunityrepo.htm" /&gt;</v>
-      </c>
-    </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>65</v>
-      </c>
-      <c r="B96" s="16" t="s">
-        <v>348</v>
+        <v>61</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>344</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="F96" s="3"/>
       <c r="H96" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributorsrepor.htm" /&gt;</v>
+        <f>CONCATENATE("&lt;item key=""",C96,""" anchor=""",B96,""" /&gt;")</f>
+        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="specificentrymediaso.htm" /&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:8">
-      <c r="A97" t="s">
-        <v>66</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>64</v>
+      <c r="A97" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>270</v>
       </c>
       <c r="F97" s="3"/>
       <c r="H97" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
+        <f t="shared" ref="H97:H119" si="3">CONCATENATE("&lt;item key=""",C97,""" anchor=""",B97,""" /&gt;")</f>
+        <v>&lt;item key="" anchor="userandcommunityrepo.htm" /&gt;</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>273</v>
+        <v>347</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F98" s="3"/>
       <c r="H98" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributorsrepor.htm" /&gt;</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>68</v>
-      </c>
-      <c r="B99" s="14" t="s">
-        <v>349</v>
+        <v>65</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>271</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F99" s="3"/>
       <c r="H99" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="specificsyndicatorre.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>69</v>
-      </c>
-      <c r="B100" s="14" t="s">
-        <v>350</v>
+        <v>66</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>64</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F100" s="3"/>
       <c r="H100" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_map_drilldown" anchor="specificgeographicre.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
       </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
+        <v>67</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="C101" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B101" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>103</v>
-      </c>
       <c r="D101" s="8" t="s">
-        <v>64</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F101" s="3"/>
       <c r="H101" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="specificsyndicatorre.htm" /&gt;</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>108</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>351</v>
+        <v>68</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_user_drilldown" anchor="specificuserengageme.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_drilldown" anchor="specificgeographicre.htm" /&gt;</v>
       </c>
     </row>
     <row r="103" spans="1:8">
-      <c r="A103" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="8"/>
+      <c r="A103" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H103" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
+      </c>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
-        <v>354</v>
-      </c>
-      <c r="B104" s="6"/>
+        <v>107</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>350</v>
+      </c>
       <c r="C104" s="6" t="s">
-        <v>353</v>
+        <v>106</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>356</v>
+        <v>63</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="3"/>
+        <v>&lt;item key="section_analytics_user_drilldown" anchor="specificuserengageme.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="8"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>353</v>
+      </c>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="H106" t="str">
+        <f t="shared" si="3"/>
         <v>&lt;item key="section_analytics_platform" anchor="" /&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
-      <c r="A105" t="s">
-        <v>358</v>
-      </c>
-      <c r="B105" s="6"/>
-      <c r="C105" s="6" t="s">
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
         <v>357</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="B107" s="6"/>
+      <c r="C107" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="H105" t="str">
+      <c r="D107" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="H107" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_analytics_os" anchor="" /&gt;</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
-      <c r="A106" t="s">
-        <v>360</v>
-      </c>
-      <c r="B106" s="6"/>
-      <c r="C106" s="6" t="s">
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
         <v>359</v>
       </c>
-      <c r="D106" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="H106" t="str">
+      <c r="B108" s="6"/>
+      <c r="C108" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="H108" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_analytics_browsers" anchor="" /&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
-      <c r="A107" t="s">
-        <v>362</v>
-      </c>
-      <c r="B107" s="6"/>
-      <c r="C107" s="6" t="s">
+    <row r="109" spans="1:8">
+      <c r="A109" t="s">
         <v>361</v>
       </c>
-      <c r="D107" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="H107" t="str">
+      <c r="B109" s="6"/>
+      <c r="C109" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="H109" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_analytics_platform_drilldown" anchor="" /&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="18.75">
-      <c r="A108" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8">
-      <c r="H109" t="str">
+    <row r="110" spans="1:8" ht="18.75">
+      <c r="A110" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="H111" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="" anchor="" /&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
-      <c r="A110" t="s">
-        <v>22</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D110" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H110" t="str">
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
+        <v>21</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D112" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H112" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_admin_users" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
-      <c r="A111" t="s">
-        <v>90</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="C111" s="5" t="s">
+    <row r="113" spans="1:8">
+      <c r="A113" t="s">
         <v>89</v>
       </c>
-      <c r="D111" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H111" t="str">
+      <c r="B113" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H113" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
-      <c r="A112" t="s">
-        <v>56</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="C112" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D112" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H112" t="str">
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>55</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H114" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
-      <c r="A113" t="s">
-        <v>23</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H113" t="str">
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
+        <v>22</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H115" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_role_drilldown" anchor="creatingcustomroles.htm" /&gt;</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="18.75">
-      <c r="A114" s="2" t="s">
+    <row r="116" spans="1:8" ht="18.75">
+      <c r="A116" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" t="s">
+        <v>146</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="C117" s="5" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="115" spans="1:8">
-      <c r="A115" t="s">
-        <v>147</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="C115" s="5" t="s">
+      <c r="D117" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D115" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="H115" t="str">
+      <c r="H117" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_desktop_upload" anchor="uploadmedia.htm" /&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="18.75">
-      <c r="A116" s="2" t="s">
+    <row r="118" spans="1:8" ht="18.75">
+      <c r="A118" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" t="s">
+        <v>150</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C119" s="5" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="117" spans="1:8">
-      <c r="A117" t="s">
-        <v>151</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="C117" s="5" t="s">
+      <c r="D119" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D117" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="H117" t="str">
+      <c r="H119" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_upload_menu" anchor="thekalturauploader.htm" /&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
-      <c r="H118" t="s">
-        <v>278</v>
+    <row r="120" spans="1:8">
+      <c r="H120" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fwr: updates to help anchors (gemini)
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@96470 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20520" windowHeight="10860"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="8715"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B13" authorId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0">
+    <comment ref="B42" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,36 +93,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B111" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-what is this?</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="372">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -928,9 +904,6 @@
     <t>bandwidthusagereport.htm</t>
   </si>
   <si>
-    <t>topcontent.htm</t>
-  </si>
-  <si>
     <t>contentcontributions.htm</t>
   </si>
   <si>
@@ -1021,9 +994,6 @@
     <t>addingorremovingipad.htm</t>
   </si>
   <si>
-    <t>add domain</t>
-  </si>
-  <si>
     <t>add/remove countries</t>
   </si>
   <si>
@@ -1039,30 +1009,12 @@
     <t>html wrapper</t>
   </si>
   <si>
-    <t>preview and embed - ipad/iphone</t>
-  </si>
-  <si>
-    <t>preview and embed - adaptive streaming</t>
-  </si>
-  <si>
-    <t>section_pne_ipad</t>
-  </si>
-  <si>
     <t>section_pne_stream</t>
   </si>
   <si>
     <t>embeddingaplayerwith.htm</t>
   </si>
   <si>
-    <t>mobilesupport.htm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">videodeliverysetting.htm </t>
-  </si>
-  <si>
-    <t>themixestab dz - legacy no? how do I get this tab</t>
-  </si>
-  <si>
     <t>addingorremovingadom.htm</t>
   </si>
   <si>
@@ -1156,9 +1108,6 @@
     <t>contentinteractionsr.htm</t>
   </si>
   <si>
-    <t>specificentrymediaso.htm</t>
-  </si>
-  <si>
     <t>specificentrycontent.htm</t>
   </si>
   <si>
@@ -1171,9 +1120,6 @@
     <t>specificsyndicatorre.htm</t>
   </si>
   <si>
-    <t>specificgeographicre.htm</t>
-  </si>
-  <si>
     <t>specificuserengageme.htm</t>
   </si>
   <si>
@@ -1216,9 +1162,6 @@
     <t>embedcodetypes.htm</t>
   </si>
   <si>
-    <t>preview and embed - embed types</t>
-  </si>
-  <si>
     <t>thekalturauploader.htm</t>
   </si>
   <si>
@@ -1235,13 +1178,75 @@
   </si>
   <si>
     <t>section_add_live_stream_man</t>
+  </si>
+  <si>
+    <t>platformreports.htm</t>
+  </si>
+  <si>
+    <t>operatingsystemsrepo.htm</t>
+  </si>
+  <si>
+    <t>browsersreport.htm</t>
+  </si>
+  <si>
+    <t>platformsdrilldownre.htm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">preview and embed - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delivery Type Read More</t>
+    </r>
+  </si>
+  <si>
+    <t>videodeliverysetting.htm</t>
+  </si>
+  <si>
+    <r>
+      <t>preview and embed -</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Embed Type Read More</t>
+    </r>
+  </si>
+  <si>
+    <t>topcontentreports.htm</t>
+  </si>
+  <si>
+    <t>specificentryreport.htm</t>
+  </si>
+  <si>
+    <t>restrictingaccessfor.htm</t>
+  </si>
+  <si>
+    <t>add domain  lines 74-77 do not have anchors but have pages)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restrict flavors (DRM) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1321,6 +1326,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1378,7 +1391,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1405,6 +1418,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1714,17 +1730,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H120"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32" style="5" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1744,21 +1760,21 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>302</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>304</v>
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("&lt;item key=""",C3,""" anchor=""",B3,""" /&gt;")</f>
@@ -1767,1253 +1783,1246 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>310</v>
+        <v>364</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>365</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H70" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
-        <v>&lt;item key="section_pne_ipad" anchor="mobilesupport.htm" /&gt;</v>
+        <f t="shared" ref="H4:H69" si="0">CONCATENATE("&lt;item key=""",C4,""" anchor=""",B4,""" /&gt;")</f>
+        <v>&lt;item key="section_pne_stream" anchor="videodeliverysetting.htm" /&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>366</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>311</v>
+        <v>353</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>308</v>
+        <v>352</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_pne_stream" anchor="videodeliverysetting.htm " /&gt;</v>
+        <v>&lt;item key="section_pne_embed" anchor="embedcodetypes.htm" /&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>364</v>
+      <c r="A6" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>363</v>
+        <v>309</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>304</v>
+        <v>72</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_entries" anchor="entriestable.htm" /&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
+      <c r="A7" t="s">
+        <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>72</v>
+        <v>239</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_entries" anchor="entriestable.htm" /&gt;</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="" anchor="editentrymenus.htm" /&gt;</v>
+        <v>&lt;item key="entry_accesscontrol" anchor="creatinganaccessprof.htm" /&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_accesscontrol" anchor="creatinganaccessprof.htm" /&gt;</v>
+        <v>&lt;item key="entry_ads" anchor="addingamidroll.htm" /&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_ads" anchor="addingamidroll.htm" /&gt;</v>
+        <v>&lt;item key="entry_captions" anchor="addingcaptionstoanen.htm" /&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>242</v>
+        <v>292</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_captions" anchor="addingcaptionstoanen.htm" /&gt;</v>
+        <v>&lt;item key="entry_clips" anchor="clippingandtrimmingm.htm" /&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>293</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="B12" s="13"/>
       <c r="C12" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="entry_clips" anchor="clippingandtrimmingm.htm" /&gt;</v>
-      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>183</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>312</v>
+        <v>184</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_content" anchor="themixestab dz - legacy no? how do I get this tab" /&gt;</v>
+        <v>&lt;item key="entry_metadata" anchor="uploadamediafileands.htm" /&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_metadata" anchor="uploadamediafileands.htm" /&gt;</v>
+        <v>&lt;item key="entry_distribution" anchor="addingadistributorto.htm" /&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_distribution" anchor="addingadistributorto.htm" /&gt;</v>
+        <v>&lt;item key="entry_flavors" anchor="theflavorstab.htm" /&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_flavors" anchor="theflavorstab.htm" /&gt;</v>
+        <v>&lt;item key="entry_replacement" anchor="replacingmedia.htm" /&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>173</v>
+        <v>83</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_replacement" anchor="replacingmedia.htm" /&gt;</v>
+        <v>&lt;item key="section_live_stream" anchor="configuringthelivest.htm" /&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>83</v>
+        <v>175</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_live_stream" anchor="configuringthelivest.htm" /&gt;</v>
+        <v>&lt;item key="entry_related" anchor="uploadingandmodifyin.htm" /&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_related" anchor="uploadingandmodifyin.htm" /&gt;</v>
+        <v>&lt;item key="entry_scheduling" anchor="contentscheduling.htm" /&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>247</v>
+        <v>310</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_scheduling" anchor="contentscheduling.htm" /&gt;</v>
+        <v>&lt;item key="entry_thumbnails" anchor="choosingathumbnailfo.htm" /&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>318</v>
+        <v>278</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_thumbnails" anchor="choosingathumbnailfo.htm" /&gt;</v>
+        <v>&lt;item key="entry_users" anchor="userstab.htm" /&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>279</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>178</v>
+        <v>115</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>36</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F22" s="3"/>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="entry_users" anchor="userstab.htm" /&gt;</v>
+        <v>&lt;item key="section_download" anchor="downloadfiles.htm" /&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>280</v>
+        <v>311</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="3"/>
+        <v>113</v>
+      </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_download" anchor="downloadfiles.htm" /&gt;</v>
+        <v>&lt;item key="section_add_entry_tags" anchor="editaddtagstoandentr.htm" /&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_entry_tags" anchor="editaddtagstoandentr.htm" /&gt;</v>
+        <v>&lt;item key="section_remove_entry_tags" anchor="editremovetagsfroman.htm" /&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_remove_entry_tags" anchor="editremovetagsfroman.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_access_control" anchor="setaccesscontrol.htm" /&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>281</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_access_control" anchor="setaccesscontrol.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_sched" anchor="setscheduling.htm" /&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>282</v>
+        <v>313</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>119</v>
+        <v>218</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>51</v>
+        <v>220</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_sched" anchor="setscheduling.htm" /&gt;</v>
+        <v>&lt;item key="section_entry_owner" anchor="changeentryowner.htm" /&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entry_owner" anchor="changeentryowner.htm" /&gt;</v>
+        <v>&lt;item key="section_entry_remove_cats" anchor="editremovecategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>223</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>322</v>
+        <v>355</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>282</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>221</v>
+        <v>111</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>222</v>
+        <v>32</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_entry_remove_cats" anchor="editremovecategories.htm" /&gt;</v>
+        <v>&lt;item key="section_add_live_stream" anchor="creatingalivestreami.htm" /&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>366</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>283</v>
+        <v>356</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>282</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>111</v>
+        <v>358</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_live_stream" anchor="creatingalivestreami.htm" /&gt;</v>
+        <v>&lt;item key="section_add_live_stream_ak" anchor="creatingalivestreami.htm" /&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>367</v>
-      </c>
-      <c r="B31" s="6"/>
+        <v>357</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>282</v>
+      </c>
       <c r="C31" s="5" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_live_stream_ak" anchor="" /&gt;</v>
+        <v>&lt;item key="section_add_live_stream_man" anchor="creatingalivestreami.htm" /&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>368</v>
-      </c>
-      <c r="B32" s="6"/>
+        <v>155</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="C32" s="5" t="s">
-        <v>370</v>
+        <v>153</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>32</v>
+        <v>154</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_live_stream_man" anchor="" /&gt;</v>
+        <v>&lt;item key="section_flavor_dropfolder" anchor="matchfilesfromdropfo.htm" /&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>155</v>
+      <c r="A33" s="14" t="s">
+        <v>159</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_dropfolder" anchor="matchfilesfromdropfo.htm" /&gt;</v>
+        <v>&lt;item key="section_flavor_upload" anchor="uploadfromdesktop.htm" /&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="14" t="s">
-        <v>159</v>
+      <c r="A34" t="s">
+        <v>161</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>248</v>
+        <v>315</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>162</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_upload" anchor="uploadfromdesktop.htm" /&gt;</v>
+        <v>&lt;item key="section_flavor_import" anchor="importfiles.htm" /&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>323</v>
+        <v>294</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>162</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_import" anchor="importfiles.htm" /&gt;</v>
+        <v>&lt;item key="section_flavor_link" anchor="linktoremotestorage.htm" /&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>160</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>295</v>
+      <c r="A36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>316</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>158</v>
+        <v>73</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>162</v>
+        <v>25</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_flavor_link" anchor="linktoremotestorage.htm" /&gt;</v>
+        <v>&lt;item key="section_moderation" anchor="themoderationtab.htm" /&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_moderation" anchor="themoderationtab.htm" /&gt;</v>
+        <f>CONCATENATE("&lt;item key=""",C37,""" anchor=""",B37,""" /&gt;")</f>
+        <v>&lt;item key="section_playlists" anchor="playliststab.htm" /&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="1" t="s">
-        <v>4</v>
+      <c r="A38" t="s">
+        <v>8</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>325</v>
+        <v>249</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H38" t="str">
-        <f>CONCATENATE("&lt;item key=""",C38,""" anchor=""",B38,""" /&gt;")</f>
-        <v>&lt;item key="section_playlists" anchor="playliststab.htm" /&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_manual_playlist" anchor="creatingamanualplayl.htm" /&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_manual_playlist" anchor="creatingamanualplayl.htm" /&gt;</v>
+        <v>&lt;item key="section_rule_playlist" anchor="creatingarulebasedpl.htm" /&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>250</v>
+        <v>23</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>251</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_rule_playlist" anchor="creatingarulebasedpl.htm" /&gt;</v>
+        <v>&lt;item key="section_edit_rule" anchor="definingarule.htm" /&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>251</v>
+      <c r="A41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_edit_rule" anchor="definingarule.htm" /&gt;</v>
+        <v>&lt;item key="section_syndication" anchor="settingupsyndication.htm" /&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>253</v>
+      <c r="A42" t="s">
+        <v>252</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>318</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_syndication" anchor="settingupsyndication.htm" /&gt;</v>
+        <v>&lt;item key="section_ExternalSyndicationPopup" anchor="googlewebmastertasks.htm" /&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>252</v>
+        <v>10</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>326</v>
+        <v>254</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_ExternalSyndicationPopup" anchor="googlewebmastertasks.htm" /&gt;</v>
+        <v>&lt;item key="section_ExternalSyndicationNotification" anchor="kmcpublishertasksfor.htm" /&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" t="s">
-        <v>10</v>
+      <c r="A44" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>254</v>
+        <v>319</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_ExternalSyndicationNotification" anchor="kmcpublishertasksfor.htm" /&gt;</v>
+        <v>&lt;item key="section_categories" anchor="categoriestable.htm" /&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="1" t="s">
-        <v>164</v>
+      <c r="A45" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>25</v>
+        <v>201</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_categories" anchor="categoriestable.htm" /&gt;</v>
+        <v>&lt;item key="section_category_parent" anchor="addingeditingaspecif.htm" /&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>328</v>
+        <v>255</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>201</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_parent" anchor="addingeditingaspecif.htm" /&gt;</v>
+        <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>255</v>
+        <v>199</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>321</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>201</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
+        <v>&lt;item key="section_category_users" anchor="editingtheentitlemen.htm" /&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>329</v>
+        <v>200</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>322</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>201</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_users" anchor="editingtheentitlemen.htm" /&gt;</v>
+        <v>&lt;item key="section_category_subcats" anchor="reorderingsubcategor.htm" /&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="4" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_category_subcats" anchor="reorderingsubcategor.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_user_permission" anchor="categorysentitlement.htm" /&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>207</v>
+        <v>320</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_permission" anchor="categorysentitlement.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_user_add" anchor="addingeditingaspecif.htm" /&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>328</v>
+        <v>284</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_user_add" anchor="addingeditingaspecif.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>211</v>
+        <v>113</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_cat_user_permission" anchor="addinguserpermission.htm" /&gt;</v>
+        <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>286</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_add_cat_tags" anchor="addtags.htm" /&gt;</v>
+        <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="4" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>287</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>114</v>
+        <v>225</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_remove_cat_tags" anchor="removetags.htm" /&gt;</v>
+        <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="4" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>288</v>
+        <v>327</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cat_move" anchor="movecategories.htm" /&gt;</v>
+        <v>&lt;item key="section_cats_list" anchor="changecategorylistin.htm" /&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_list" anchor="changecategorylistin.htm" /&gt;</v>
+        <v>&lt;item key="section_cats_access" anchor="changecontentprivacy.htm" /&gt;</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_access" anchor="changecontentprivacy.htm" /&gt;</v>
+        <v>&lt;item key="section_cats_owner" anchor="changecategoryowner.htm" /&gt;</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="4" t="s">
-        <v>235</v>
+        <v>306</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>231</v>
+        <v>307</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>232</v>
+        <v>308</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_owner" anchor="changecategoryowner.htm" /&gt;</v>
+        <v>&lt;item key="section_cats_cont" anchor="changecontributionpo.htm" /&gt;</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="H59" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_cats_cont" anchor="changecontributionpo.htm" /&gt;</v>
-      </c>
+      <c r="A59" s="4"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="4"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="8"/>
+      <c r="A60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_uploads" anchor="youruploads.htm" /&gt;</v>
+      </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>289</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_uploads" anchor="youruploads.htm" /&gt;</v>
+        <v>&lt;item key="section_bulk_log" anchor="bulkuploadlog.htm" /&gt;</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>290</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_bulk_log" anchor="bulkuploadlog.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H63" t="str">
-        <f t="shared" si="0"/>
         <v>&lt;item key="section_drop_folders" anchor="usingadropfolder.htm" /&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="18.75">
-      <c r="A64" s="2" t="s">
+    <row r="63" spans="1:8" ht="18.75">
+      <c r="A63" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_studio_player_list" anchor="playerlist.htm" /&gt;</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_studio_player_list" anchor="playerlist.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" t="s">
-        <v>122</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H66" t="str">
-        <f t="shared" si="0"/>
         <v>&lt;item key="section_studio_player" anchor="editingaplayer.htm" /&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="18.75">
-      <c r="A67" s="2" t="s">
+    <row r="66" spans="1:8" ht="18.75">
+      <c r="A66" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;item key="section_acc_overview" anchor="accountsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_acc_overview" anchor="accountsettings.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_integration" anchor="integrationsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>152</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>259</v>
+        <v>328</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>44</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;item key="section_acc_integration" anchor="integrationsettings.htm" /&gt;</v>
+        <v>&lt;item key="section_entitlement_more" anchor="entitlementsettings.htm" /&gt;</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>151</v>
+        <v>236</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>44</v>
+        <v>237</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;item key="section_entitlement_more" anchor="entitlementsettings.htm" /&gt;</v>
+        <f t="shared" ref="H70:H74" si="1">CONCATENATE("&lt;item key=""",C70,""" anchor=""",B70,""" /&gt;")</f>
+        <v>&lt;item key="section_cat_entitlement" anchor="editingtheentitlemen.htm" /&gt;</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>238</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>329</v>
+        <v>15</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>295</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>237</v>
+        <v>125</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" ref="H71:H75" si="1">CONCATENATE("&lt;item key=""",C71,""" anchor=""",B71,""" /&gt;")</f>
-        <v>&lt;item key="section_cat_entitlement" anchor="editingtheentitlemen.htm" /&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;item key="section_acc_access_control" anchor="accesscontrolprofile.htm" /&gt;</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>296</v>
+        <v>329</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>46</v>
+        <v>82</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_acc_access_control" anchor="accesscontrolprofile.htm" /&gt;</v>
+        <v>&lt;item key="section_access_control_profile" anchor="editinganaccessprofi.htm" /&gt;</v>
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" t="s">
-        <v>17</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="A73" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D73" s="8"/>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="section_access_control_profile" anchor="editinganaccessprofi.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="addingorremovingadom.htm" /&gt;</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="D74" s="8"/>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="addingorremovingadom.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="addingorremovinggeog.htm" /&gt;</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>297</v>
       </c>
       <c r="D75" s="8"/>
       <c r="H75" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;item key="" anchor="addingorremovinggeog.htm" /&gt;</v>
+        <f>CONCATENATE("&lt;item key=""",C75,""" anchor=""",B75,""" /&gt;")</f>
+        <v>&lt;item key="" anchor="addingorremovingipad.htm" /&gt;</v>
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>298</v>
+      <c r="A76" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>369</v>
       </c>
       <c r="D76" s="8"/>
       <c r="H76" t="str">
         <f>CONCATENATE("&lt;item key=""",C76,""" anchor=""",B76,""" /&gt;")</f>
-        <v>&lt;item key="" anchor="addingorremovingipad.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="restrictingaccessfor.htm" /&gt;</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3075,7 +3084,7 @@
         <v>139</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>137</v>
@@ -3127,7 +3136,7 @@
         <v>85</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>84</v>
@@ -3204,15 +3213,15 @@
         <v>62</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>268</v>
+        <v>333</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>367</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>90</v>
@@ -3222,7 +3231,7 @@
       </c>
       <c r="H89" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_top_content" anchor="topcontent.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_content" anchor="topcontentreports.htm" /&gt;</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -3230,7 +3239,7 @@
         <v>56</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>91</v>
@@ -3248,7 +3257,7 @@
         <v>57</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>92</v>
@@ -3266,7 +3275,7 @@
         <v>58</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>93</v>
@@ -3283,8 +3292,8 @@
       <c r="A93" t="s">
         <v>59</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>344</v>
+      <c r="B93" s="16" t="s">
+        <v>368</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>94</v>
@@ -3294,7 +3303,7 @@
       </c>
       <c r="H93" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;item key="section_analytics_video_drilldown" anchor="specificentrymediaso.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_video_drilldown" anchor="specificentryreport.htm" /&gt;</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -3302,7 +3311,7 @@
         <v>60</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>95</v>
@@ -3321,7 +3330,7 @@
         <v>70</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>96</v>
@@ -3339,8 +3348,8 @@
       <c r="A96" t="s">
         <v>61</v>
       </c>
-      <c r="B96" s="6" t="s">
-        <v>344</v>
+      <c r="B96" s="16" t="s">
+        <v>268</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>97</v>
@@ -3351,7 +3360,7 @@
       <c r="F96" s="3"/>
       <c r="H96" t="str">
         <f>CONCATENATE("&lt;item key=""",C96,""" anchor=""",B96,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="specificentrymediaso.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="contentcontributions.htm" /&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -3359,20 +3368,16 @@
         <v>20</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F97" s="3"/>
-      <c r="H97" t="str">
-        <f t="shared" ref="H97:H119" si="3">CONCATENATE("&lt;item key=""",C97,""" anchor=""",B97,""" /&gt;")</f>
-        <v>&lt;item key="" anchor="userandcommunityrepo.htm" /&gt;</v>
-      </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>64</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>99</v>
@@ -3382,7 +3387,7 @@
       </c>
       <c r="F98" s="3"/>
       <c r="H98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="H98:H118" si="3">CONCATENATE("&lt;item key=""",C98,""" anchor=""",B98,""" /&gt;")</f>
         <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributorsrepor.htm" /&gt;</v>
       </c>
     </row>
@@ -3391,7 +3396,7 @@
         <v>65</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>100</v>
@@ -3410,7 +3415,7 @@
         <v>66</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>101</v>
@@ -3429,7 +3434,7 @@
         <v>67</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>104</v>
@@ -3448,7 +3453,7 @@
         <v>68</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>349</v>
+        <v>270</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>105</v>
@@ -3458,7 +3463,7 @@
       </c>
       <c r="H102" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_map_drilldown" anchor="specificgeographicre.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_drilldown" anchor="geographicdistributi.htm" /&gt;</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3466,7 +3471,7 @@
         <v>103</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>102</v>
@@ -3484,7 +3489,7 @@
         <v>107</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>106</v>
@@ -3499,7 +3504,7 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
@@ -3507,66 +3512,74 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>353</v>
-      </c>
-      <c r="B106" s="6"/>
+        <v>343</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>360</v>
+      </c>
       <c r="C106" s="6" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="H106" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_platform" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_platform" anchor="platformreports.htm" /&gt;</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>357</v>
-      </c>
-      <c r="B107" s="6"/>
+        <v>347</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>361</v>
+      </c>
       <c r="C107" s="6" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_os" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_os" anchor="operatingsystemsrepo.htm" /&gt;</v>
       </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>359</v>
-      </c>
-      <c r="B108" s="6"/>
+        <v>349</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>362</v>
+      </c>
       <c r="C108" s="6" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_browsers" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_browsers" anchor="browsersreport.htm" /&gt;</v>
       </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>361</v>
-      </c>
-      <c r="B109" s="6"/>
+        <v>351</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>363</v>
+      </c>
       <c r="C109" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_analytics_platform_drilldown" anchor="" /&gt;</v>
+        <v>&lt;item key="section_analytics_platform_drilldown" anchor="platformsdrilldownre.htm" /&gt;</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="18.75">
@@ -3575,132 +3588,126 @@
       </c>
     </row>
     <row r="111" spans="1:8">
+      <c r="A111" t="s">
+        <v>21</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="H111" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="" anchor="" /&gt;</v>
+        <v>&lt;item key="section_admin_users" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D112" s="10" t="s">
-        <v>54</v>
+        <v>88</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_admin_users" anchor="addingauser.htm" /&gt;</v>
+        <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
     <row r="113" spans="1:8">
       <c r="A113" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>274</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
+      </c>
+      <c r="D113" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
+        <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
       </c>
     </row>
     <row r="114" spans="1:8">
       <c r="A114" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>275</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D114" s="10" t="s">
-        <v>53</v>
+        <v>87</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="H114" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8">
-      <c r="A115" t="s">
-        <v>22</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H115" t="str">
-        <f t="shared" si="3"/>
         <v>&lt;item key="section_role_drilldown" anchor="creatingcustomroles.htm" /&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="18.75">
-      <c r="A116" s="2" t="s">
+    <row r="115" spans="1:8" ht="18.75">
+      <c r="A115" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
-      <c r="A117" t="s">
+    <row r="116" spans="1:8">
+      <c r="A116" t="s">
         <v>146</v>
       </c>
-      <c r="B117" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="C117" s="5" t="s">
+      <c r="B116" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="C116" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D117" s="7" t="s">
+      <c r="D116" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="H117" t="str">
+      <c r="H116" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_desktop_upload" anchor="uploadmedia.htm" /&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="18.75">
-      <c r="A118" s="2" t="s">
+    <row r="117" spans="1:8" ht="18.75">
+      <c r="A117" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
-      <c r="A119" t="s">
+    <row r="118" spans="1:8">
+      <c r="A118" t="s">
         <v>150</v>
       </c>
-      <c r="B119" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="C119" s="5" t="s">
+      <c r="B118" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="C118" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D119" s="7" t="s">
+      <c r="D118" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="H119" t="str">
+      <c r="H118" t="str">
         <f t="shared" si="3"/>
         <v>&lt;item key="section_upload_menu" anchor="thekalturauploader.htm" /&gt;</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
-      <c r="H120" t="s">
-        <v>277</v>
+    <row r="119" spans="1:8">
+      <c r="H119" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fwr: fix analytics / distributions / drilldown anchor
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@96586 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="373">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -1240,6 +1240,9 @@
   </si>
   <si>
     <t xml:space="preserve">restrict flavors (DRM) </t>
+  </si>
+  <si>
+    <t>specificentrymediaso.htm</t>
   </si>
 </sst>
 </file>
@@ -1732,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H119"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2543,7 +2546,7 @@
         <v>&lt;item key="section_category_metadata" anchor="addingmetadatatoacat.htm" /&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" ht="30">
       <c r="A47" s="4" t="s">
         <v>199</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>&lt;item key="section_cat_entitlement" anchor="editingtheentitlemen.htm" /&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" ht="30">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -2955,7 +2958,7 @@
         <v>&lt;item key="section_acc_access_control" anchor="accesscontrolprofile.htm" /&gt;</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" ht="30">
       <c r="A72" t="s">
         <v>17</v>
       </c>
@@ -3349,7 +3352,7 @@
         <v>61</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>268</v>
+        <v>372</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>97</v>
@@ -3360,7 +3363,7 @@
       <c r="F96" s="3"/>
       <c r="H96" t="str">
         <f>CONCATENATE("&lt;item key=""",C96,""" anchor=""",B96,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="contentcontributions.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="specificentrymediaso.htm" /&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:8">

</xml_diff>

<commit_message>
FEC-1463 update uiconf to reflect new help links
</commit_message>
<xml_diff>
--- a/KMC/docs/help.xlsx
+++ b/KMC/docs/help.xlsx
@@ -69,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B101" authorId="0" shapeId="0">
+    <comment ref="B102" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8626" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8635" uniqueCount="393">
   <si>
     <t xml:space="preserve">location </t>
   </si>
@@ -1279,6 +1279,30 @@
   </si>
   <si>
     <t>section_add_live_stream_mul</t>
+  </si>
+  <si>
+    <t>live</t>
+  </si>
+  <si>
+    <t>live reports</t>
+  </si>
+  <si>
+    <t>section_analytics_live</t>
+  </si>
+  <si>
+    <t>livereports.htm</t>
+  </si>
+  <si>
+    <t>analytics.view.LiveContent.mxml</t>
+  </si>
+  <si>
+    <t>transcoding settings - live profiles list</t>
+  </si>
+  <si>
+    <t>section_acc_live_transcoding_profiles</t>
+  </si>
+  <si>
+    <t>cloudtranscodingprofilefeatures.htm</t>
   </si>
 </sst>
 </file>
@@ -1772,16 +1796,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD123"/>
+  <dimension ref="A1:XFD126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="27" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="7" customWidth="1"/>
   </cols>
@@ -35883,7 +35907,7 @@
         <v>43</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" ref="H81:H99" si="2049">CONCATENATE("&lt;item key=""",C81,""" anchor=""",B81,""" /&gt;")</f>
+        <f t="shared" ref="H81:H100" si="2049">CONCATENATE("&lt;item key=""",C81,""" anchor=""",B81,""" /&gt;")</f>
         <v>&lt;item key="section_acc_transcoding_def" anchor="convertingvideosinto.htm" /&gt;</v>
       </c>
     </row>
@@ -35907,277 +35931,276 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>140</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>262</v>
+        <v>390</v>
+      </c>
+      <c r="B83" t="s">
+        <v>392</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>141</v>
+        <v>391</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_transcoding_profile_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_live_transcoding_profiles" anchor="cloudtranscodingprofilefeatures.htm" /&gt;</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>330</v>
+        <v>262</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_transcoding_flavor_edit" anchor="editingoptionsforfla.htm" /&gt;</v>
+        <v>&lt;item key="section_transcoding_profile_edit" anchor="editingandcreatingtr.htm" /&gt;</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>47</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>130</v>
+        <v>139</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_acc_custom_data" anchor="addingaschema.htm" /&gt;</v>
+        <v>&lt;item key="section_transcoding_flavor_edit" anchor="editingoptionsforfla.htm" /&gt;</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>142</v>
+        <v>47</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="C86" s="6"/>
+        <v>264</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="D86" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="" anchor="kalturacustommetadat.htm" /&gt;</v>
+        <v>&lt;item key="section_acc_custom_data" anchor="addingaschema.htm" /&gt;</v>
       </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>84</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="C87" s="6"/>
       <c r="D87" s="8" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_custom_data_field" anchor="addingcustomdatafiel.htm" /&gt;</v>
+        <v>&lt;item key="" anchor="kalturacustommetadat.htm" /&gt;</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>42</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>131</v>
+        <v>85</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_acc_user" anchor="myusersettings.htm" /&gt;</v>
+        <v>&lt;item key="section_custom_data_field" anchor="addingcustomdatafiel.htm" /&gt;</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>134</v>
+        <v>41</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="2049"/>
+        <v>&lt;item key="section_acc_user" anchor="myusersettings.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>133</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H90" t="str">
+        <f t="shared" si="2049"/>
         <v>&lt;item key="section_acc_upgrade" anchor="accountupgrade.htm" /&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="18.75">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:8" ht="18.75">
+      <c r="A91" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="A91" t="s">
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
         <v>19</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B92" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C92" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D92" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H91" t="str">
+      <c r="H92" t="str">
         <f t="shared" si="2049"/>
         <v>&lt;item key="section_analytics_usage" anchor="bandwidthusagereport.htm" /&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:8">
+      <c r="A93" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B93" s="5" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="4" t="s">
+    <row r="94" spans="1:8">
+      <c r="A94" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="B93" s="16" t="s">
+      <c r="B94" s="16" t="s">
         <v>367</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C94" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D93" s="8" t="s">
+      <c r="D94" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H93" t="str">
+      <c r="H94" t="str">
         <f t="shared" si="2049"/>
         <v>&lt;item key="section_analytics_top_content" anchor="topcontentreports.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="A94" t="s">
-        <v>56</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H94" t="str">
-        <f t="shared" si="2049"/>
-        <v>&lt;item key="section_analytics_content_dropoff" anchor="contentdropoffreport.htm" /&gt;</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>38</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_analytics_content_interactions" anchor="contentinteractionsr.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_content_dropoff" anchor="contentdropoffreport.htm" /&gt;</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>268</v>
+        <v>335</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>38</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_analytics_content_contribution" anchor="contentcontributions.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_content_interactions" anchor="contentinteractionsr.htm" /&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>59</v>
-      </c>
-      <c r="B97" s="16" t="s">
-        <v>368</v>
+        <v>58</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>268</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>38</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_analytics_video_drilldown" anchor="specificentryreport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_content_contribution" anchor="contentcontributions.htm" /&gt;</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>60</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>336</v>
+        <v>59</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>368</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F98" s="3"/>
       <c r="H98" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="specificentrycontent.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_video_drilldown" anchor="specificentryreport.htm" /&gt;</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>38</v>
@@ -36185,84 +36208,84 @@
       <c r="F99" s="3"/>
       <c r="H99" t="str">
         <f t="shared" si="2049"/>
-        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="specificcontentinter.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_video_drilldown_dropoff" anchor="specificentrycontent.htm" /&gt;</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>61</v>
-      </c>
-      <c r="B100" s="16" t="s">
-        <v>372</v>
+        <v>70</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>337</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>38</v>
       </c>
       <c r="F100" s="3"/>
       <c r="H100" t="str">
-        <f>CONCATENATE("&lt;item key=""",C100,""" anchor=""",B100,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="specificentrymediaso.htm" /&gt;</v>
+        <f t="shared" si="2049"/>
+        <v>&lt;item key="section_analytics_video_drilldown_interactions" anchor="specificcontentinter.htm" /&gt;</v>
       </c>
     </row>
     <row r="101" spans="1:8">
-      <c r="A101" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>269</v>
+      <c r="A101" t="s">
+        <v>61</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="F101" s="3"/>
+      <c r="H101" t="str">
+        <f>CONCATENATE("&lt;item key=""",C101,""" anchor=""",B101,""" /&gt;")</f>
+        <v>&lt;item key="section_analytics_drilldown_contribution" anchor="specificentrymediaso.htm" /&gt;</v>
+      </c>
     </row>
     <row r="102" spans="1:8">
-      <c r="A102" t="s">
-        <v>64</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D102" s="8" t="s">
-        <v>63</v>
+      <c r="A102" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="F102" s="3"/>
-      <c r="H102" t="str">
-        <f t="shared" ref="H102:H122" si="2050">CONCATENATE("&lt;item key=""",C102,""" anchor=""",B102,""" /&gt;")</f>
-        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributorsrepor.htm" /&gt;</v>
-      </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>270</v>
+        <v>338</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>63</v>
       </c>
       <c r="F103" s="3"/>
       <c r="H103" t="str">
-        <f t="shared" si="2050"/>
-        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
+        <f t="shared" ref="H103:H125" si="2050">CONCATENATE("&lt;item key=""",C103,""" anchor=""",B103,""" /&gt;")</f>
+        <v>&lt;item key="section_analytics_top_contributors" anchor="topcontributorsrepor.htm" /&gt;</v>
       </c>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>63</v>
@@ -36270,18 +36293,18 @@
       <c r="F104" s="3"/>
       <c r="H104" t="str">
         <f t="shared" si="2050"/>
-        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_overlay" anchor="geographicdistributi.htm" /&gt;</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>67</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>339</v>
+        <v>66</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>271</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>63</v>
@@ -36289,268 +36312,313 @@
       <c r="F105" s="3"/>
       <c r="H105" t="str">
         <f t="shared" si="2050"/>
-        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="specificsyndicatorre.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_top_syndications" anchor="topsyndications.htm" /&gt;</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>270</v>
+        <v>339</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>63</v>
       </c>
+      <c r="F106" s="3"/>
       <c r="H106" t="str">
         <f t="shared" si="2050"/>
-        <v>&lt;item key="section_analytics_map_drilldown" anchor="geographicdistributi.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_syndication_drilldown" anchor="specificsyndicatorre.htm" /&gt;</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>103</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>272</v>
+        <v>68</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>270</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>63</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="2050"/>
-        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_map_drilldown" anchor="geographicdistributi.htm" /&gt;</v>
       </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>340</v>
+        <v>272</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>63</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="2050"/>
-        <v>&lt;item key="section_analytics_user_drilldown" anchor="specificuserengageme.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_user_engagement" anchor="userengagementreport.htm" /&gt;</v>
       </c>
     </row>
     <row r="109" spans="1:8">
-      <c r="A109" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="B109" s="6"/>
-      <c r="C109" s="6"/>
-      <c r="D109" s="8"/>
+      <c r="A109" t="s">
+        <v>107</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H109" t="str">
+        <f t="shared" si="2050"/>
+        <v>&lt;item key="section_analytics_user_drilldown" anchor="specificuserengageme.htm" /&gt;</v>
+      </c>
     </row>
     <row r="110" spans="1:8">
-      <c r="A110" t="s">
-        <v>343</v>
-      </c>
-      <c r="B110" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="D110" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="H110" t="str">
-        <f t="shared" si="2050"/>
-        <v>&lt;item key="section_analytics_platform" anchor="platformreports.htm" /&gt;</v>
-      </c>
+      <c r="A110" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="8"/>
     </row>
     <row r="111" spans="1:8">
       <c r="A111" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D111" s="8" t="s">
         <v>345</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="2050"/>
-        <v>&lt;item key="section_analytics_os" anchor="operatingsystemsrepo.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_platform" anchor="platformreports.htm" /&gt;</v>
       </c>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>345</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="2050"/>
-        <v>&lt;item key="section_analytics_browsers" anchor="browsersreport.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_os" anchor="operatingsystemsrepo.htm" /&gt;</v>
       </c>
     </row>
     <row r="113" spans="1:8">
       <c r="A113" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>345</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="2050"/>
+        <v>&lt;item key="section_analytics_browsers" anchor="browsersreport.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>351</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="H114" t="str">
+        <f t="shared" si="2050"/>
         <v>&lt;item key="section_analytics_platform_drilldown" anchor="platformsdrilldownre.htm" /&gt;</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="18.75">
-      <c r="A114" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="115" spans="1:8">
-      <c r="A115" t="s">
-        <v>21</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D115" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H115" t="str">
-        <f t="shared" si="2050"/>
-        <v>&lt;item key="section_admin_users" anchor="addingauser.htm" /&gt;</v>
-      </c>
+      <c r="A115" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B115" s="16"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="8"/>
     </row>
     <row r="116" spans="1:8">
       <c r="A116" t="s">
-        <v>89</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="C116" s="5" t="s">
-        <v>88</v>
+        <v>386</v>
+      </c>
+      <c r="B116" t="s">
+        <v>388</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>387</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>39</v>
+        <v>389</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="2050"/>
-        <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
+        <v>&lt;item key="section_analytics_live" anchor="livereports.htm" /&gt;</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
-      <c r="A117" t="s">
-        <v>55</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D117" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H117" t="str">
-        <f t="shared" si="2050"/>
-        <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
+    <row r="117" spans="1:8" ht="18.75">
+      <c r="A117" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="118" spans="1:8">
       <c r="A118" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>40</v>
+        <v>135</v>
+      </c>
+      <c r="D118" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="2050"/>
-        <v>&lt;item key="section_role_drilldown" anchor="creatingcustomroles.htm" /&gt;</v>
+        <v>&lt;item key="section_admin_users" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="18.75">
-      <c r="A119" s="2" t="s">
-        <v>143</v>
+    <row r="119" spans="1:8">
+      <c r="A119" t="s">
+        <v>89</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H119" t="str">
+        <f t="shared" si="2050"/>
+        <v>&lt;item key="section_user_drilldown" anchor="addingauser.htm" /&gt;</v>
       </c>
     </row>
     <row r="120" spans="1:8">
       <c r="A120" t="s">
-        <v>146</v>
+        <v>55</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>341</v>
+        <v>274</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>145</v>
+        <v>136</v>
+      </c>
+      <c r="D120" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="H120" t="str">
         <f t="shared" si="2050"/>
+        <v>&lt;item key="section_admin_roles" anchor="rolemanagement.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" t="s">
+        <v>22</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H121" t="str">
+        <f t="shared" si="2050"/>
+        <v>&lt;item key="section_role_drilldown" anchor="creatingcustomroles.htm" /&gt;</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="18.75">
+      <c r="A122" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" t="s">
+        <v>146</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H123" t="str">
+        <f t="shared" si="2050"/>
         <v>&lt;item key="section_desktop_upload" anchor="uploadmedia.htm" /&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="18.75">
-      <c r="A121" s="2" t="s">
+    <row r="124" spans="1:8" ht="18.75">
+      <c r="A124" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
-      <c r="A122" t="s">
+    <row r="125" spans="1:8">
+      <c r="A125" t="s">
         <v>150</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B125" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="C122" s="5" t="s">
+      <c r="C125" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D122" s="7" t="s">
+      <c r="D125" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="H122" t="str">
+      <c r="H125" t="str">
         <f t="shared" si="2050"/>
         <v>&lt;item key="section_upload_menu" anchor="thekalturauploader.htm" /&gt;</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
-      <c r="H123" t="s">
+    <row r="126" spans="1:8">
+      <c r="H126" t="s">
         <v>276</v>
       </c>
     </row>

</xml_diff>